<commit_message>
Relative Strength Index (RSI) Service.
</commit_message>
<xml_diff>
--- a/sources/Services/Indicators.xlsx
+++ b/sources/Services/Indicators.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MA for S&amp;P 500 (^GSPC)" sheetId="1" r:id="rId1"/>
     <sheet name="BB for S&amp;P 500 (^GSPC)" sheetId="2" r:id="rId2"/>
+    <sheet name="RSI for S&amp;P 500" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -59,6 +60,24 @@
   </si>
   <si>
     <t>SMMA</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Gain (U)</t>
+  </si>
+  <si>
+    <t>Loss (D)</t>
+  </si>
+  <si>
+    <t>Gain (U) EMA</t>
+  </si>
+  <si>
+    <t>Loss (D) EMA</t>
+  </si>
+  <si>
+    <t>RSI</t>
   </si>
 </sst>
 </file>
@@ -664,7 +683,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -709,6 +728,7 @@
     <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,8 +1088,8 @@
   <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,7 +4601,7 @@
         <v>4</v>
       </c>
       <c r="I102" s="38">
-        <f t="shared" ref="I102:I133" si="10">((I101 * COUNT(C93:C102))-I101+C102)/COUNT(C93:C102)</f>
+        <f t="shared" ref="I102:I112" si="10">((I101 * COUNT(C93:C102))-I101+C102)/COUNT(C93:C102)</f>
         <v>1725.825979135539</v>
       </c>
       <c r="J102" s="7" t="s">
@@ -4968,8 +4988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9195,4 +9215,4525 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="2" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="2.5703125" style="32" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="37" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="42"/>
+    <col min="8" max="8" width="13.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>41435</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="31">
+        <v>1642.81</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="34">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0</v>
+      </c>
+      <c r="H2" s="42">
+        <v>0</v>
+      </c>
+      <c r="I2" s="42">
+        <v>0</v>
+      </c>
+      <c r="J2" s="42">
+        <v>0</v>
+      </c>
+      <c r="K2" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>41436</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1626.13</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="34">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="42">
+        <f>IF(C3&gt;C2,C3-C2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="42">
+        <v>0</v>
+      </c>
+      <c r="I3" s="42">
+        <f>IF(C2&gt;C3,C2-C3,0)</f>
+        <v>16.679999999999836</v>
+      </c>
+      <c r="J3" s="42">
+        <v>0</v>
+      </c>
+      <c r="K3" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>41437</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="31">
+        <v>1612.52</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="34">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="42">
+        <f>IF(C4&gt;C3,C4-C3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0</v>
+      </c>
+      <c r="I4" s="42">
+        <f>IF(C3&gt;C4,C3-C4,0)</f>
+        <v>13.610000000000127</v>
+      </c>
+      <c r="J4" s="42">
+        <v>0</v>
+      </c>
+      <c r="K4" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>41438</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1636.36</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="34">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="42">
+        <f>IF(C5&gt;C4,C5-C4,0)</f>
+        <v>23.839999999999918</v>
+      </c>
+      <c r="H5" s="42">
+        <v>0</v>
+      </c>
+      <c r="I5" s="42">
+        <f>IF(C4&gt;C5,C4-C5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="42">
+        <v>0</v>
+      </c>
+      <c r="K5" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>41439</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="31">
+        <v>1626.73</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="34">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="42">
+        <f>IF(C6&gt;C5,C6-C5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="42">
+        <v>0</v>
+      </c>
+      <c r="I6" s="42">
+        <f>IF(C5&gt;C6,C5-C6,0)</f>
+        <v>9.6299999999998818</v>
+      </c>
+      <c r="J6" s="42">
+        <v>0</v>
+      </c>
+      <c r="K6" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>41442</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31">
+        <v>1639.04</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="34">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="42">
+        <f>IF(C7&gt;C6,C7-C6,0)</f>
+        <v>12.309999999999945</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0</v>
+      </c>
+      <c r="I7" s="42">
+        <f>IF(C6&gt;C7,C6-C7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="42">
+        <v>0</v>
+      </c>
+      <c r="K7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>41443</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="31">
+        <v>1651.81</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="34">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="42">
+        <f>IF(C8&gt;C7,C8-C7,0)</f>
+        <v>12.769999999999982</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0</v>
+      </c>
+      <c r="I8" s="42">
+        <f>IF(C7&gt;C8,C7-C8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="42">
+        <v>0</v>
+      </c>
+      <c r="K8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>41444</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="31">
+        <v>1628.93</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="42">
+        <f>IF(C9&gt;C8,C9-C8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="42">
+        <v>0</v>
+      </c>
+      <c r="I9" s="42">
+        <f>IF(C8&gt;C9,C8-C9,0)</f>
+        <v>22.879999999999882</v>
+      </c>
+      <c r="J9" s="42">
+        <v>0</v>
+      </c>
+      <c r="K9" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>41445</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="31">
+        <v>1588.19</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="34">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="42">
+        <f>IF(C10&gt;C9,C10-C9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="42">
+        <v>0</v>
+      </c>
+      <c r="I10" s="42">
+        <f>IF(C9&gt;C10,C9-C10,0)</f>
+        <v>40.740000000000009</v>
+      </c>
+      <c r="J10" s="42">
+        <v>0</v>
+      </c>
+      <c r="K10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>41446</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="31">
+        <v>1592.43</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="34">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="42">
+        <f>IF(C11&gt;C10,C11-C10,0)</f>
+        <v>4.2400000000000091</v>
+      </c>
+      <c r="H11" s="42">
+        <v>0</v>
+      </c>
+      <c r="I11" s="42">
+        <f>IF(C10&gt;C11,C10-C11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="42">
+        <v>0</v>
+      </c>
+      <c r="K11" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="22">
+        <v>41449</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="31">
+        <v>1573.09</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="34">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="42">
+        <f>IF(C12&gt;C11,C12-C11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="42">
+        <f>IF(C11&gt;C12,C11-C12,0)</f>
+        <v>19.340000000000146</v>
+      </c>
+      <c r="J12" s="42">
+        <v>0</v>
+      </c>
+      <c r="K12" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="22">
+        <v>41450</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="31">
+        <v>1588.03</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="34">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="42">
+        <f>IF(C13&gt;C12,C13-C12,0)</f>
+        <v>14.940000000000055</v>
+      </c>
+      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="I13" s="42">
+        <f>IF(C12&gt;C13,C12-C13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="42">
+        <v>0</v>
+      </c>
+      <c r="K13" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="22">
+        <v>41451</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="31">
+        <v>1603.26</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="42">
+        <f>IF(C14&gt;C13,C14-C13,0)</f>
+        <v>15.230000000000018</v>
+      </c>
+      <c r="H14" s="42">
+        <v>0</v>
+      </c>
+      <c r="I14" s="42">
+        <f>IF(C13&gt;C14,C13-C14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="42">
+        <v>0</v>
+      </c>
+      <c r="K14" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>41452</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="31">
+        <v>1613.2</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="37">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="42">
+        <f>IF(C15&gt;C14,C15-C14,0)</f>
+        <v>9.9400000000000546</v>
+      </c>
+      <c r="H15" s="42">
+        <v>0</v>
+      </c>
+      <c r="I15" s="42">
+        <f>IF(C14&gt;C15,C14-C15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="42">
+        <v>0</v>
+      </c>
+      <c r="K15" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="22">
+        <v>41453</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="31">
+        <v>1606.28</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="37">
+        <f t="shared" ref="E16:E79" si="0">100-(100 / (1 + K16))</f>
+        <v>41.811987268570405</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="42">
+        <f>IF(C16&gt;C15,C16-C15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="42">
+        <f>AVERAGE(G3:G16)</f>
+        <v>6.6621428571428556</v>
+      </c>
+      <c r="I16" s="42">
+        <f>IF(C15&gt;C16,C15-C16,0)</f>
+        <v>6.9200000000000728</v>
+      </c>
+      <c r="J16" s="42">
+        <f>AVERAGE(I3:I16)</f>
+        <v>9.2714285714285687</v>
+      </c>
+      <c r="K16" s="42">
+        <f t="shared" ref="K16:K66" si="1">H16/J16</f>
+        <v>0.71856702619414492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
+        <v>41456</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1614.96</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="37">
+        <f t="shared" si="0"/>
+        <v>46.311586248588142</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="42">
+        <f>IF(C17&gt;C16,C17-C16,0)</f>
+        <v>8.6800000000000637</v>
+      </c>
+      <c r="H17" s="42">
+        <f t="shared" ref="H17:H80" si="2">G17*2/(14+1)+H16*(1-2/(14+1))</f>
+        <v>6.9311904761904835</v>
+      </c>
+      <c r="I17" s="42">
+        <f>IF(C16&gt;C17,C16-C17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="42">
+        <f t="shared" ref="J17:J80" si="3">I17*2/(14+1)+J16*(1-2/(14+1))</f>
+        <v>8.0352380952380926</v>
+      </c>
+      <c r="K17" s="42">
+        <f t="shared" si="1"/>
+        <v>0.8625992651416392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
+        <v>41457</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="31">
+        <v>1614.08</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="37">
+        <f t="shared" si="0"/>
+        <v>45.896412506564097</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="42">
+        <f>IF(C18&gt;C17,C18-C17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="42">
+        <f t="shared" si="2"/>
+        <v>6.0070317460317524</v>
+      </c>
+      <c r="I18" s="42">
+        <f>IF(C17&gt;C18,C17-C18,0)</f>
+        <v>0.88000000000010914</v>
+      </c>
+      <c r="J18" s="42">
+        <f t="shared" si="3"/>
+        <v>7.0812063492063615</v>
+      </c>
+      <c r="K18" s="42">
+        <f t="shared" si="1"/>
+        <v>0.84830627011808535</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="22">
+        <v>41458</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="31">
+        <v>1615.41</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="37">
+        <f t="shared" si="0"/>
+        <v>46.729222887030637</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="42">
+        <f>IF(C19&gt;C18,C19-C18,0)</f>
+        <v>1.3300000000001546</v>
+      </c>
+      <c r="H19" s="42">
+        <f t="shared" si="2"/>
+        <v>5.3834275132275398</v>
+      </c>
+      <c r="I19" s="42">
+        <f>IF(C18&gt;C19,C18-C19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="42">
+        <f t="shared" si="3"/>
+        <v>6.1370455026455133</v>
+      </c>
+      <c r="K19" s="42">
+        <f t="shared" si="1"/>
+        <v>0.87720182470651242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="22">
+        <v>41460</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="31">
+        <v>1631.89</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="37">
+        <f t="shared" si="0"/>
+        <v>56.338164033492767</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="42">
+        <f>IF(C20&gt;C19,C20-C19,0)</f>
+        <v>16.480000000000018</v>
+      </c>
+      <c r="H20" s="42">
+        <f t="shared" si="2"/>
+        <v>6.8629705114638702</v>
+      </c>
+      <c r="I20" s="42">
+        <f>IF(C19&gt;C20,C19-C20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="42">
+        <f t="shared" si="3"/>
+        <v>5.3187727689594446</v>
+      </c>
+      <c r="K20" s="42">
+        <f t="shared" si="1"/>
+        <v>1.2903297075438944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="22">
+        <v>41463</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="31">
+        <v>1640.46</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="37">
+        <f t="shared" si="0"/>
+        <v>60.602280925995679</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="42">
+        <f>IF(C21&gt;C20,C21-C20,0)</f>
+        <v>8.5699999999999363</v>
+      </c>
+      <c r="H21" s="42">
+        <f t="shared" si="2"/>
+        <v>7.0905744432686788</v>
+      </c>
+      <c r="I21" s="42">
+        <f>IF(C20&gt;C21,C20-C21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="42">
+        <f t="shared" si="3"/>
+        <v>4.6096030664315188</v>
+      </c>
+      <c r="K21" s="42">
+        <f t="shared" si="1"/>
+        <v>1.5382180072953182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="22">
+        <v>41464</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="31">
+        <v>1652.32</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="37">
+        <f t="shared" si="0"/>
+        <v>65.917385186956011</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="42">
+        <f>IF(C22&gt;C21,C22-C21,0)</f>
+        <v>11.8599999999999</v>
+      </c>
+      <c r="H22" s="42">
+        <f t="shared" si="2"/>
+        <v>7.7264978508328417</v>
+      </c>
+      <c r="I22" s="42">
+        <f>IF(C21&gt;C22,C21-C22,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="42">
+        <f t="shared" si="3"/>
+        <v>3.9949893242406498</v>
+      </c>
+      <c r="K22" s="42">
+        <f t="shared" si="1"/>
+        <v>1.9340471835432154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="22">
+        <v>41465</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="31">
+        <v>1652.62</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="37">
+        <f t="shared" si="0"/>
+        <v>66.051060556366423</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="42">
+        <f>IF(C23&gt;C22,C23-C22,0)</f>
+        <v>0.29999999999995453</v>
+      </c>
+      <c r="H23" s="42">
+        <f t="shared" si="2"/>
+        <v>6.7362981373884567</v>
+      </c>
+      <c r="I23" s="42">
+        <f>IF(C22&gt;C23,C22-C23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="42">
+        <f t="shared" si="3"/>
+        <v>3.4623240810085631</v>
+      </c>
+      <c r="K23" s="42">
+        <f t="shared" si="1"/>
+        <v>1.945600117082684</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22">
+        <v>41466</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="31">
+        <v>1675.02</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="37">
+        <f t="shared" si="0"/>
+        <v>74.625277361614764</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="42">
+        <f>IF(C24&gt;C23,C24-C23,0)</f>
+        <v>22.400000000000091</v>
+      </c>
+      <c r="H24" s="42">
+        <f t="shared" si="2"/>
+        <v>8.8247917190700083</v>
+      </c>
+      <c r="I24" s="42">
+        <f>IF(C23&gt;C24,C23-C24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="42">
+        <f t="shared" si="3"/>
+        <v>3.0006808702074217</v>
+      </c>
+      <c r="K24" s="42">
+        <f t="shared" si="1"/>
+        <v>2.9409297758678337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
+        <v>41467</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="31">
+        <v>1680.19</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="37">
+        <f t="shared" si="0"/>
+        <v>76.224428962725369</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="42">
+        <f>IF(C25&gt;C24,C25-C24,0)</f>
+        <v>5.1700000000000728</v>
+      </c>
+      <c r="H25" s="42">
+        <f t="shared" si="2"/>
+        <v>8.3374861565273513</v>
+      </c>
+      <c r="I25" s="42">
+        <f>IF(C24&gt;C25,C24-C25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="42">
+        <f t="shared" si="3"/>
+        <v>2.6005900875130989</v>
+      </c>
+      <c r="K25" s="42">
+        <f t="shared" si="1"/>
+        <v>3.2059978220175216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="22">
+        <v>41470</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="31">
+        <v>1682.5</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="37">
+        <f t="shared" si="0"/>
+        <v>76.972602819597554</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="42">
+        <f>IF(C26&gt;C25,C26-C25,0)</f>
+        <v>2.3099999999999454</v>
+      </c>
+      <c r="H26" s="42">
+        <f t="shared" si="2"/>
+        <v>7.5338213356570307</v>
+      </c>
+      <c r="I26" s="42">
+        <f>IF(C25&gt;C26,C25-C26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="42">
+        <f t="shared" si="3"/>
+        <v>2.2538447425113524</v>
+      </c>
+      <c r="K26" s="42">
+        <f t="shared" si="1"/>
+        <v>3.3426531976920693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="31">
+        <v>0</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="37">
+        <f t="shared" si="0"/>
+        <v>2.80449473479527</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="42">
+        <f>IF(C27&gt;C26,C27-C26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="42">
+        <f t="shared" si="2"/>
+        <v>6.5293118242360935</v>
+      </c>
+      <c r="I27" s="42">
+        <f>IF(C26&gt;C27,C26-C27,0)</f>
+        <v>1682.5</v>
+      </c>
+      <c r="J27" s="42">
+        <f t="shared" si="3"/>
+        <v>226.28666544350986</v>
+      </c>
+      <c r="K27" s="42">
+        <f t="shared" si="1"/>
+        <v>2.8854160767445083E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>41471</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="31">
+        <v>1676.26</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="37">
+        <f t="shared" si="0"/>
+        <v>53.885126822286999</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="42">
+        <f>IF(C28&gt;C27,C28-C27,0)</f>
+        <v>1676.26</v>
+      </c>
+      <c r="H28" s="42">
+        <f t="shared" si="2"/>
+        <v>229.16007024767126</v>
+      </c>
+      <c r="I28" s="42">
+        <f>IF(C27&gt;C28,C27-C28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="42">
+        <f t="shared" si="3"/>
+        <v>196.11511005104188</v>
+      </c>
+      <c r="K28" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1684977775961727</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>41472</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="31">
+        <v>1680.91</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="37">
+        <f t="shared" si="0"/>
+        <v>53.962569548790583</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="42">
+        <f>IF(C29&gt;C28,C29-C28,0)</f>
+        <v>4.6500000000000909</v>
+      </c>
+      <c r="H29" s="42">
+        <f t="shared" si="2"/>
+        <v>199.22539421464845</v>
+      </c>
+      <c r="I29" s="42">
+        <f>IF(C28&gt;C29,C28-C29,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="42">
+        <f t="shared" si="3"/>
+        <v>169.96642871090296</v>
+      </c>
+      <c r="K29" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1721455567764636</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
+        <v>41473</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="31">
+        <v>1689.37</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="37">
+        <f t="shared" si="0"/>
+        <v>54.12429845583042</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="42">
+        <f>IF(C30&gt;C29,C30-C29,0)</f>
+        <v>8.459999999999809</v>
+      </c>
+      <c r="H30" s="42">
+        <f t="shared" si="2"/>
+        <v>173.79000831936199</v>
+      </c>
+      <c r="I30" s="42">
+        <f>IF(C29&gt;C30,C29-C30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="42">
+        <f t="shared" si="3"/>
+        <v>147.30423821611589</v>
+      </c>
+      <c r="K30" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1798031775867017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="22">
+        <v>41474</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="31">
+        <v>1692.09</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="37">
+        <f t="shared" si="0"/>
+        <v>54.184007500493628</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="42">
+        <f>IF(C31&gt;C30,C31-C30,0)</f>
+        <v>2.7200000000000273</v>
+      </c>
+      <c r="H31" s="42">
+        <f t="shared" si="2"/>
+        <v>150.9806738767804</v>
+      </c>
+      <c r="I31" s="42">
+        <f>IF(C30&gt;C31,C30-C31,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="42">
+        <f t="shared" si="3"/>
+        <v>127.66367312063377</v>
+      </c>
+      <c r="K31" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1826439752686231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="22">
+        <v>41477</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="31">
+        <v>1695.53</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="37">
+        <f t="shared" si="0"/>
+        <v>54.270861110163871</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="42">
+        <f>IF(C32&gt;C31,C32-C31,0)</f>
+        <v>3.4400000000000546</v>
+      </c>
+      <c r="H32" s="42">
+        <f t="shared" si="2"/>
+        <v>131.30858402654303</v>
+      </c>
+      <c r="I32" s="42">
+        <f>IF(C31&gt;C32,C31-C32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="42">
+        <f t="shared" si="3"/>
+        <v>110.64185003788261</v>
+      </c>
+      <c r="K32" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1867894831981241</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="22">
+        <v>41478</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1692.39</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="37">
+        <f t="shared" si="0"/>
+        <v>54.162720117233299</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="42">
+        <f>IF(C33&gt;C32,C33-C32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="42">
+        <f t="shared" si="2"/>
+        <v>113.80077282300397</v>
+      </c>
+      <c r="I33" s="42">
+        <f>IF(C32&gt;C33,C32-C33,0)</f>
+        <v>3.1399999999998727</v>
+      </c>
+      <c r="J33" s="42">
+        <f t="shared" si="3"/>
+        <v>96.308270032831587</v>
+      </c>
+      <c r="K33" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1816303291940471</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="22">
+        <v>41479</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="31">
+        <v>1685.94</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="37">
+        <f t="shared" si="0"/>
+        <v>53.908121633286683</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="42">
+        <f>IF(C34&gt;C33,C34-C33,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="42">
+        <f t="shared" si="2"/>
+        <v>98.627336446603437</v>
+      </c>
+      <c r="I34" s="42">
+        <f>IF(C33&gt;C34,C33-C34,0)</f>
+        <v>6.4500000000000455</v>
+      </c>
+      <c r="J34" s="42">
+        <f t="shared" si="3"/>
+        <v>84.327167361787374</v>
+      </c>
+      <c r="K34" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1695796210426979</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="22">
+        <v>41480</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="31">
+        <v>1690.25</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="37">
+        <f t="shared" si="0"/>
+        <v>54.074567900384231</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="42">
+        <f>IF(C35&gt;C34,C35-C34,0)</f>
+        <v>4.3099999999999454</v>
+      </c>
+      <c r="H35" s="42">
+        <f t="shared" si="2"/>
+        <v>86.051691587056311</v>
+      </c>
+      <c r="I35" s="42">
+        <f>IF(C34&gt;C35,C34-C35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="42">
+        <f t="shared" si="3"/>
+        <v>73.083545046882392</v>
+      </c>
+      <c r="K35" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1774427681614921</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
+        <v>41481</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1691.65</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="37">
+        <f t="shared" si="0"/>
+        <v>54.136642534619092</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="42">
+        <f>IF(C36&gt;C35,C36-C35,0)</f>
+        <v>1.4000000000000909</v>
+      </c>
+      <c r="H36" s="42">
+        <f t="shared" si="2"/>
+        <v>74.764799375448817</v>
+      </c>
+      <c r="I36" s="42">
+        <f>IF(C35&gt;C36,C35-C36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="42">
+        <f t="shared" si="3"/>
+        <v>63.33907237396474</v>
+      </c>
+      <c r="K36" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1803898695267374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="22">
+        <v>41484</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="31">
+        <v>1685.33</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="37">
+        <f t="shared" si="0"/>
+        <v>53.758163098504149</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="42">
+        <f>IF(C37&gt;C36,C37-C36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="42">
+        <f t="shared" si="2"/>
+        <v>64.796159458722315</v>
+      </c>
+      <c r="I37" s="42">
+        <f>IF(C36&gt;C37,C36-C37,0)</f>
+        <v>6.3200000000001637</v>
+      </c>
+      <c r="J37" s="42">
+        <f t="shared" si="3"/>
+        <v>55.736529390769462</v>
+      </c>
+      <c r="K37" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1625438499127867</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="22">
+        <v>41485</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="31">
+        <v>1685.96</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="37">
+        <f t="shared" si="0"/>
+        <v>53.795317334876913</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="42">
+        <f>IF(C38&gt;C37,C38-C37,0)</f>
+        <v>0.63000000000010914</v>
+      </c>
+      <c r="H38" s="42">
+        <f t="shared" si="2"/>
+        <v>56.240671530892691</v>
+      </c>
+      <c r="I38" s="42">
+        <f>IF(C37&gt;C38,C37-C38,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="42">
+        <f t="shared" si="3"/>
+        <v>48.304992138666869</v>
+      </c>
+      <c r="K38" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1642828006150014</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
+        <v>41486</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="31">
+        <v>1685.73</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="37">
+        <f t="shared" si="0"/>
+        <v>53.77711588590882</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="42">
+        <f>IF(C39&gt;C38,C39-C38,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="42">
+        <f t="shared" si="2"/>
+        <v>48.741915326773665</v>
+      </c>
+      <c r="I39" s="42">
+        <f>IF(C38&gt;C39,C38-C39,0)</f>
+        <v>0.23000000000001819</v>
+      </c>
+      <c r="J39" s="42">
+        <f t="shared" si="3"/>
+        <v>41.894993186844623</v>
+      </c>
+      <c r="K39" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1634305586205236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="22">
+        <v>41487</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="31">
+        <v>1706.87</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="37">
+        <f t="shared" si="0"/>
+        <v>55.37826932652532</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="42">
+        <f>IF(C40&gt;C39,C40-C39,0)</f>
+        <v>21.139999999999873</v>
+      </c>
+      <c r="H40" s="42">
+        <f t="shared" si="2"/>
+        <v>45.061659949870496</v>
+      </c>
+      <c r="I40" s="42">
+        <f>IF(C39&gt;C40,C39-C40,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="42">
+        <f t="shared" si="3"/>
+        <v>36.308994095265341</v>
+      </c>
+      <c r="K40" s="42">
+        <f t="shared" si="1"/>
+        <v>1.2410605436118787</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
+        <v>41488</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="31">
+        <v>1709.67</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="37">
+        <f t="shared" si="0"/>
+        <v>55.613248961695895</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="42">
+        <f>IF(C41&gt;C40,C41-C40,0)</f>
+        <v>2.8000000000001819</v>
+      </c>
+      <c r="H41" s="42">
+        <f t="shared" si="2"/>
+        <v>39.426771956554454</v>
+      </c>
+      <c r="I41" s="42">
+        <f>IF(C40&gt;C41,C40-C41,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="42">
+        <f t="shared" si="3"/>
+        <v>31.467794882563297</v>
+      </c>
+      <c r="K41" s="42">
+        <f t="shared" si="1"/>
+        <v>1.2529245250165695</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="22">
+        <v>41491</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="31">
+        <v>1707.14</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="37">
+        <f t="shared" si="0"/>
+        <v>55.309584056078585</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="42">
+        <f>IF(C42&gt;C41,C42-C41,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="42">
+        <f t="shared" si="2"/>
+        <v>34.16986902901386</v>
+      </c>
+      <c r="I42" s="42">
+        <f>IF(C41&gt;C42,C41-C42,0)</f>
+        <v>2.5299999999999727</v>
+      </c>
+      <c r="J42" s="42">
+        <f t="shared" si="3"/>
+        <v>27.609422231554856</v>
+      </c>
+      <c r="K42" s="42">
+        <f t="shared" si="1"/>
+        <v>1.2376162290698376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="22">
+        <v>41492</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="31">
+        <v>1697.37</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="37">
+        <f t="shared" si="0"/>
+        <v>53.995875960034823</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="42">
+        <f>IF(C43&gt;C42,C43-C42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="42">
+        <f t="shared" si="2"/>
+        <v>29.613886491812014</v>
+      </c>
+      <c r="I43" s="42">
+        <f>IF(C42&gt;C43,C42-C43,0)</f>
+        <v>9.7700000000002092</v>
+      </c>
+      <c r="J43" s="42">
+        <f t="shared" si="3"/>
+        <v>25.230832600680905</v>
+      </c>
+      <c r="K43" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1737181630309268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="22">
+        <v>41493</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="31">
+        <v>1690.91</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="37">
+        <f t="shared" si="0"/>
+        <v>53.034827025312218</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="42">
+        <f>IF(C44&gt;C43,C44-C43,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="42">
+        <f t="shared" si="2"/>
+        <v>25.665368292903747</v>
+      </c>
+      <c r="I44" s="42">
+        <f>IF(C43&gt;C44,C43-C44,0)</f>
+        <v>6.459999999999809</v>
+      </c>
+      <c r="J44" s="42">
+        <f t="shared" si="3"/>
+        <v>22.728054920590093</v>
+      </c>
+      <c r="K44" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1292373404841012</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="22">
+        <v>41494</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="31">
+        <v>1697.48</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="37">
+        <f t="shared" si="0"/>
+        <v>53.995695919467792</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="42">
+        <f>IF(C45&gt;C44,C45-C44,0)</f>
+        <v>6.5699999999999363</v>
+      </c>
+      <c r="H45" s="42">
+        <f t="shared" si="2"/>
+        <v>23.119319187183237</v>
+      </c>
+      <c r="I45" s="42">
+        <f>IF(C44&gt;C45,C44-C45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="42">
+        <f t="shared" si="3"/>
+        <v>19.69764759784475</v>
+      </c>
+      <c r="K45" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1737096560562326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="22">
+        <v>41495</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="31">
+        <v>1691.42</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="37">
+        <f t="shared" si="0"/>
+        <v>52.845034491166736</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="42">
+        <f>IF(C46&gt;C45,C46-C45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="42">
+        <f t="shared" si="2"/>
+        <v>20.036743295558807</v>
+      </c>
+      <c r="I46" s="42">
+        <f>IF(C45&gt;C46,C45-C46,0)</f>
+        <v>6.0599999999999454</v>
+      </c>
+      <c r="J46" s="42">
+        <f t="shared" si="3"/>
+        <v>17.879294584798775</v>
+      </c>
+      <c r="K46" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1206674402352723</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="22">
+        <v>41498</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="31">
+        <v>1689.47</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="37">
+        <f t="shared" si="0"/>
+        <v>52.430195297292606</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="42">
+        <f>IF(C47&gt;C46,C47-C46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="42">
+        <f t="shared" si="2"/>
+        <v>17.365177522817632</v>
+      </c>
+      <c r="I47" s="42">
+        <f>IF(C46&gt;C47,C46-C47,0)</f>
+        <v>1.9500000000000455</v>
+      </c>
+      <c r="J47" s="42">
+        <f t="shared" si="3"/>
+        <v>15.755388640158944</v>
+      </c>
+      <c r="K47" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1021738606025555</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="22">
+        <v>41499</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="31">
+        <v>1694.16</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="37">
+        <f t="shared" si="0"/>
+        <v>53.444418380688347</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="42">
+        <f>IF(C48&gt;C47,C48-C47,0)</f>
+        <v>4.6900000000000546</v>
+      </c>
+      <c r="H48" s="42">
+        <f t="shared" si="2"/>
+        <v>15.675153853108622</v>
+      </c>
+      <c r="I48" s="42">
+        <f>IF(C47&gt;C48,C47-C48,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="42">
+        <f t="shared" si="3"/>
+        <v>13.654670154804419</v>
+      </c>
+      <c r="K48" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1479701578579173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="22">
+        <v>41500</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="31">
+        <v>1685.39</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="37">
+        <f t="shared" si="0"/>
+        <v>51.093992194266569</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="42">
+        <f>IF(C49&gt;C48,C49-C48,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="42">
+        <f t="shared" si="2"/>
+        <v>13.585133339360807</v>
+      </c>
+      <c r="I49" s="42">
+        <f>IF(C48&gt;C49,C48-C49,0)</f>
+        <v>8.7699999999999818</v>
+      </c>
+      <c r="J49" s="42">
+        <f t="shared" si="3"/>
+        <v>13.003380800830495</v>
+      </c>
+      <c r="K49" s="42">
+        <f t="shared" si="1"/>
+        <v>1.0447385604898347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="22">
+        <v>41501</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="31">
+        <v>1661.32</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="37">
+        <f t="shared" si="0"/>
+        <v>44.847869862584453</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="42">
+        <f>IF(C50&gt;C49,C50-C49,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="42">
+        <f t="shared" si="2"/>
+        <v>11.773782227446032</v>
+      </c>
+      <c r="I50" s="42">
+        <f>IF(C49&gt;C50,C49-C50,0)</f>
+        <v>24.070000000000164</v>
+      </c>
+      <c r="J50" s="42">
+        <f t="shared" si="3"/>
+        <v>14.478930027386451</v>
+      </c>
+      <c r="K50" s="42">
+        <f t="shared" si="1"/>
+        <v>0.81316659485032983</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="22">
+        <v>41502</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="31">
+        <v>1655.83</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="37">
+        <f t="shared" si="0"/>
+        <v>43.449975525652732</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="42">
+        <f>IF(C51&gt;C50,C51-C50,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="42">
+        <f t="shared" si="2"/>
+        <v>10.203944597119895</v>
+      </c>
+      <c r="I51" s="42">
+        <f>IF(C50&gt;C51,C50-C51,0)</f>
+        <v>5.4900000000000091</v>
+      </c>
+      <c r="J51" s="42">
+        <f t="shared" si="3"/>
+        <v>13.280406023734926</v>
+      </c>
+      <c r="K51" s="42">
+        <f t="shared" si="1"/>
+        <v>0.76834583060813522</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="22">
+        <v>41505</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="31">
+        <v>1646.06</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="37">
+        <f t="shared" si="0"/>
+        <v>40.836314899482119</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="42">
+        <f>IF(C52&gt;C51,C52-C51,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="42">
+        <f t="shared" si="2"/>
+        <v>8.8434186508372417</v>
+      </c>
+      <c r="I52" s="42">
+        <f>IF(C51&gt;C52,C51-C52,0)</f>
+        <v>9.7699999999999818</v>
+      </c>
+      <c r="J52" s="42">
+        <f t="shared" si="3"/>
+        <v>12.812351887236932</v>
+      </c>
+      <c r="K52" s="42">
+        <f t="shared" si="1"/>
+        <v>0.69022602006791922</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="22">
+        <v>41506</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="31">
+        <v>1652.35</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="37">
+        <f t="shared" si="0"/>
+        <v>43.366972710658636</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="42">
+        <f>IF(C53&gt;C52,C53-C52,0)</f>
+        <v>6.2899999999999636</v>
+      </c>
+      <c r="H53" s="42">
+        <f t="shared" si="2"/>
+        <v>8.502962830725604</v>
+      </c>
+      <c r="I53" s="42">
+        <f>IF(C52&gt;C53,C52-C53,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="42">
+        <f t="shared" si="3"/>
+        <v>11.104038302272009</v>
+      </c>
+      <c r="K53" s="42">
+        <f t="shared" si="1"/>
+        <v>0.76575409767686087</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="22">
+        <v>41507</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="31">
+        <v>1642.8</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="37">
+        <f t="shared" si="0"/>
+        <v>40.343847373526913</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="42">
+        <f>IF(C54&gt;C53,C54-C53,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="42">
+        <f t="shared" si="2"/>
+        <v>7.3692344532955234</v>
+      </c>
+      <c r="I54" s="42">
+        <f>IF(C53&gt;C54,C53-C54,0)</f>
+        <v>9.5499999999999545</v>
+      </c>
+      <c r="J54" s="42">
+        <f t="shared" si="3"/>
+        <v>10.896833195302403</v>
+      </c>
+      <c r="K54" s="42">
+        <f t="shared" si="1"/>
+        <v>0.6762730346714293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="22">
+        <v>41508</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="31">
+        <v>1656.96</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="37">
+        <f t="shared" si="0"/>
+        <v>46.700493341760897</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="42">
+        <f>IF(C55&gt;C54,C55-C54,0)</f>
+        <v>14.160000000000082</v>
+      </c>
+      <c r="H55" s="42">
+        <f t="shared" si="2"/>
+        <v>8.274669859522799</v>
+      </c>
+      <c r="I55" s="42">
+        <f>IF(C54&gt;C55,C54-C55,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="42">
+        <f t="shared" si="3"/>
+        <v>9.4439221025954154</v>
+      </c>
+      <c r="K55" s="42">
+        <f t="shared" si="1"/>
+        <v>0.87618997378734431</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="22">
+        <v>41509</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="31">
+        <v>1663.5</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="37">
+        <f t="shared" si="0"/>
+        <v>49.564484349777594</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="42">
+        <f>IF(C56&gt;C55,C56-C55,0)</f>
+        <v>6.5399999999999636</v>
+      </c>
+      <c r="H56" s="42">
+        <f t="shared" si="2"/>
+        <v>8.0433805449197546</v>
+      </c>
+      <c r="I56" s="42">
+        <f>IF(C55&gt;C56,C55-C56,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J56" s="42">
+        <f t="shared" si="3"/>
+        <v>8.1847324889160262</v>
+      </c>
+      <c r="K56" s="42">
+        <f t="shared" si="1"/>
+        <v>0.98272980281424049</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="22">
+        <v>41512</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="31">
+        <v>1656.78</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="37">
+        <f t="shared" si="0"/>
+        <v>46.595988656139781</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="42">
+        <f>IF(C57&gt;C56,C57-C56,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="42">
+        <f t="shared" si="2"/>
+        <v>6.9709298055971205</v>
+      </c>
+      <c r="I57" s="42">
+        <f>IF(C56&gt;C57,C56-C57,0)</f>
+        <v>6.7200000000000273</v>
+      </c>
+      <c r="J57" s="42">
+        <f t="shared" si="3"/>
+        <v>7.9894348237272261</v>
+      </c>
+      <c r="K57" s="42">
+        <f t="shared" si="1"/>
+        <v>0.87251851468825758</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="22">
+        <v>41513</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="31">
+        <v>1630.48</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="37">
+        <f t="shared" si="0"/>
+        <v>36.676521344984188</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="42">
+        <f>IF(C58&gt;C57,C58-C57,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="42">
+        <f t="shared" si="2"/>
+        <v>6.041472498184171</v>
+      </c>
+      <c r="I58" s="42">
+        <f>IF(C57&gt;C58,C57-C58,0)</f>
+        <v>26.299999999999955</v>
+      </c>
+      <c r="J58" s="42">
+        <f t="shared" si="3"/>
+        <v>10.430843513896924</v>
+      </c>
+      <c r="K58" s="42">
+        <f t="shared" si="1"/>
+        <v>0.57919309115654627</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="22">
+        <v>41514</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="31">
+        <v>1634.96</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="37">
+        <f t="shared" si="0"/>
+        <v>39.219677300558757</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="42">
+        <f>IF(C59&gt;C58,C59-C58,0)</f>
+        <v>4.4800000000000182</v>
+      </c>
+      <c r="H59" s="42">
+        <f t="shared" si="2"/>
+        <v>5.8332761650929505</v>
+      </c>
+      <c r="I59" s="42">
+        <f>IF(C58&gt;C59,C58-C59,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="42">
+        <f t="shared" si="3"/>
+        <v>9.0400643787106674</v>
+      </c>
+      <c r="K59" s="42">
+        <f t="shared" si="1"/>
+        <v>0.64526931675733457</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="22">
+        <v>41515</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="31">
+        <v>1638.17</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="37">
+        <f t="shared" si="0"/>
+        <v>41.172938439713015</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="42">
+        <f>IF(C60&gt;C59,C60-C59,0)</f>
+        <v>3.2100000000000364</v>
+      </c>
+      <c r="H60" s="42">
+        <f t="shared" si="2"/>
+        <v>5.483506009747229</v>
+      </c>
+      <c r="I60" s="42">
+        <f>IF(C59&gt;C60,C59-C60,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="42">
+        <f t="shared" si="3"/>
+        <v>7.8347224615492452</v>
+      </c>
+      <c r="K60" s="42">
+        <f t="shared" si="1"/>
+        <v>0.69989792703683285</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="22">
+        <v>41516</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="31">
+        <v>1632.97</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="37">
+        <f t="shared" si="0"/>
+        <v>38.839901343824032</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="42">
+        <f>IF(C61&gt;C60,C61-C60,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="42">
+        <f t="shared" si="2"/>
+        <v>4.7523718751142656</v>
+      </c>
+      <c r="I61" s="42">
+        <f>IF(C60&gt;C61,C60-C61,0)</f>
+        <v>5.2000000000000455</v>
+      </c>
+      <c r="J61" s="42">
+        <f t="shared" si="3"/>
+        <v>7.4834261333426859</v>
+      </c>
+      <c r="K61" s="42">
+        <f t="shared" si="1"/>
+        <v>0.63505295441347309</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="22">
+        <v>41520</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="31">
+        <v>1639.77</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="37">
+        <f t="shared" si="0"/>
+        <v>43.65718069709132</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="42">
+        <f>IF(C62&gt;C61,C62-C61,0)</f>
+        <v>6.7999999999999545</v>
+      </c>
+      <c r="H62" s="42">
+        <f t="shared" si="2"/>
+        <v>5.0253889584323579</v>
+      </c>
+      <c r="I62" s="42">
+        <f>IF(C61&gt;C62,C61-C62,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="42">
+        <f t="shared" si="3"/>
+        <v>6.4856359822303284</v>
+      </c>
+      <c r="K62" s="42">
+        <f t="shared" si="1"/>
+        <v>0.77484906217388261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="22">
+        <v>41521</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="31">
+        <v>1653.08</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="37">
+        <f t="shared" si="0"/>
+        <v>52.166301107745269</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="42">
+        <f>IF(C63&gt;C62,C63-C62,0)</f>
+        <v>13.309999999999945</v>
+      </c>
+      <c r="H63" s="42">
+        <f t="shared" si="2"/>
+        <v>6.1300037639747034</v>
+      </c>
+      <c r="I63" s="42">
+        <f>IF(C62&gt;C63,C62-C63,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J63" s="42">
+        <f t="shared" si="3"/>
+        <v>5.6208845179329519</v>
+      </c>
+      <c r="K63" s="42">
+        <f t="shared" si="1"/>
+        <v>1.0905763575852607</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="22">
+        <v>41522</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="31">
+        <v>1655.08</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="37">
+        <f t="shared" si="0"/>
+        <v>53.386847845253548</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="42">
+        <f>IF(C64&gt;C63,C64-C63,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H64" s="42">
+        <f t="shared" si="2"/>
+        <v>5.5793365954447429</v>
+      </c>
+      <c r="I64" s="42">
+        <f>IF(C63&gt;C64,C63-C64,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J64" s="42">
+        <f t="shared" si="3"/>
+        <v>4.871433248875225</v>
+      </c>
+      <c r="K64" s="42">
+        <f t="shared" si="1"/>
+        <v>1.145317262990921</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="22">
+        <v>41523</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="31">
+        <v>1655.17</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="37">
+        <f t="shared" si="0"/>
+        <v>53.448523579566491</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="42">
+        <f>IF(C65&gt;C64,C65-C64,0)</f>
+        <v>9.0000000000145519E-2</v>
+      </c>
+      <c r="H65" s="42">
+        <f t="shared" si="2"/>
+        <v>4.8474250493854631</v>
+      </c>
+      <c r="I65" s="42">
+        <f>IF(C64&gt;C65,C64-C65,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J65" s="42">
+        <f t="shared" si="3"/>
+        <v>4.2219088156918616</v>
+      </c>
+      <c r="K65" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1481595792331425</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="22">
+        <v>41526</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="31">
+        <v>1671.71</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="37">
+        <f t="shared" si="0"/>
+        <v>63.647948471932835</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="42">
+        <f>IF(C66&gt;C65,C66-C65,0)</f>
+        <v>16.539999999999964</v>
+      </c>
+      <c r="H66" s="42">
+        <f t="shared" si="2"/>
+        <v>6.4064350428007302</v>
+      </c>
+      <c r="I66" s="42">
+        <f>IF(C65&gt;C66,C65-C66,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="42">
+        <f t="shared" si="3"/>
+        <v>3.6589876402662802</v>
+      </c>
+      <c r="K66" s="42">
+        <f t="shared" si="1"/>
+        <v>1.7508763823904325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="22">
+        <v>41527</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="31">
+        <v>1683.99</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="37">
+        <f t="shared" si="0"/>
+        <v>69.392775333332693</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" s="42">
+        <f>IF(C67&gt;C66,C67-C66,0)</f>
+        <v>12.279999999999973</v>
+      </c>
+      <c r="H67" s="42">
+        <f t="shared" si="2"/>
+        <v>7.1895770370939625</v>
+      </c>
+      <c r="I67" s="42">
+        <f>IF(C66&gt;C67,C66-C67,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="42">
+        <f t="shared" si="3"/>
+        <v>3.1711226215641095</v>
+      </c>
+      <c r="K67" s="42">
+        <f t="shared" ref="K67:K111" si="4">H67/J67</f>
+        <v>2.2672024689943431</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="22">
+        <v>41528</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="31">
+        <v>1689.13</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="37">
+        <f t="shared" si="0"/>
+        <v>71.563184608167234</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="42">
+        <f>IF(C68&gt;C67,C68-C67,0)</f>
+        <v>5.1400000000001</v>
+      </c>
+      <c r="H68" s="42">
+        <f t="shared" si="2"/>
+        <v>6.9163000988147809</v>
+      </c>
+      <c r="I68" s="42">
+        <f>IF(C67&gt;C68,C67-C68,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J68" s="42">
+        <f t="shared" si="3"/>
+        <v>2.7483062720222282</v>
+      </c>
+      <c r="K68" s="42">
+        <f t="shared" si="4"/>
+        <v>2.5165681748147035</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="22">
+        <v>41529</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="31">
+        <v>1683.42</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="37">
+        <f t="shared" si="0"/>
+        <v>65.600451010230984</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="42">
+        <f>IF(C69&gt;C68,C69-C68,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="42">
+        <f t="shared" si="2"/>
+        <v>5.9941267523061432</v>
+      </c>
+      <c r="I69" s="42">
+        <f>IF(C68&gt;C69,C68-C69,0)</f>
+        <v>5.7100000000000364</v>
+      </c>
+      <c r="J69" s="42">
+        <f t="shared" si="3"/>
+        <v>3.1431987690859362</v>
+      </c>
+      <c r="K69" s="42">
+        <f t="shared" si="4"/>
+        <v>1.9070148573675079</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="22">
+        <v>41530</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="31">
+        <v>1687.99</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="37">
+        <f t="shared" si="0"/>
+        <v>68.058229459379092</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="42">
+        <f>IF(C70&gt;C69,C70-C69,0)</f>
+        <v>4.5699999999999363</v>
+      </c>
+      <c r="H70" s="42">
+        <f t="shared" si="2"/>
+        <v>5.8042431853319822</v>
+      </c>
+      <c r="I70" s="42">
+        <f>IF(C69&gt;C70,C69-C70,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J70" s="42">
+        <f t="shared" si="3"/>
+        <v>2.7241055998744783</v>
+      </c>
+      <c r="K70" s="42">
+        <f t="shared" si="4"/>
+        <v>2.1306968370093404</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="22">
+        <v>41533</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="31">
+        <v>1697.6</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="37">
+        <f t="shared" si="0"/>
+        <v>72.777483416154524</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="42">
+        <f>IF(C71&gt;C70,C71-C70,0)</f>
+        <v>9.6099999999999</v>
+      </c>
+      <c r="H71" s="42">
+        <f t="shared" si="2"/>
+        <v>6.3116774272877052</v>
+      </c>
+      <c r="I71" s="42">
+        <f>IF(C70&gt;C71,C70-C71,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J71" s="42">
+        <f t="shared" si="3"/>
+        <v>2.3608915198912146</v>
+      </c>
+      <c r="K71" s="42">
+        <f t="shared" si="4"/>
+        <v>2.6734296659164309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="22">
+        <v>41534</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="31">
+        <v>1704.76</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="37">
+        <f t="shared" si="0"/>
+        <v>75.84545144464478</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="42">
+        <f>IF(C72&gt;C71,C72-C71,0)</f>
+        <v>7.1600000000000819</v>
+      </c>
+      <c r="H72" s="42">
+        <f t="shared" si="2"/>
+        <v>6.424787103649356</v>
+      </c>
+      <c r="I72" s="42">
+        <f>IF(C71&gt;C72,C71-C72,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J72" s="42">
+        <f t="shared" si="3"/>
+        <v>2.0461059839057194</v>
+      </c>
+      <c r="K72" s="42">
+        <f t="shared" si="4"/>
+        <v>3.1400069958181587</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="22">
+        <v>41535</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="31">
+        <v>1725.52</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="37">
+        <f t="shared" si="0"/>
+        <v>82.459050806351925</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="42">
+        <f>IF(C73&gt;C72,C73-C72,0)</f>
+        <v>20.759999999999991</v>
+      </c>
+      <c r="H73" s="42">
+        <f t="shared" si="2"/>
+        <v>8.3361488231627732</v>
+      </c>
+      <c r="I73" s="42">
+        <f>IF(C72&gt;C73,C72-C73,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="42">
+        <f t="shared" si="3"/>
+        <v>1.7732918527182902</v>
+      </c>
+      <c r="K73" s="42">
+        <f t="shared" si="4"/>
+        <v>4.7009457638821486</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="22">
+        <v>41536</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="31">
+        <v>1722.34</v>
+      </c>
+      <c r="D74" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="37">
+        <f t="shared" si="0"/>
+        <v>78.652771400017727</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="42">
+        <f>IF(C74&gt;C73,C74-C73,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H74" s="42">
+        <f t="shared" si="2"/>
+        <v>7.2246623134077366</v>
+      </c>
+      <c r="I74" s="42">
+        <f>IF(C73&gt;C74,C73-C74,0)</f>
+        <v>3.1800000000000637</v>
+      </c>
+      <c r="J74" s="42">
+        <f t="shared" si="3"/>
+        <v>1.9608529390225269</v>
+      </c>
+      <c r="K74" s="42">
+        <f t="shared" si="4"/>
+        <v>3.6844488281763681</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="22">
+        <v>41537</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="31">
+        <v>1709.91</v>
+      </c>
+      <c r="D75" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="37">
+        <f t="shared" si="0"/>
+        <v>65.099815967359021</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="42">
+        <f>IF(C75&gt;C74,C75-C74,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H75" s="42">
+        <f t="shared" si="2"/>
+        <v>6.2613740049533719</v>
+      </c>
+      <c r="I75" s="42">
+        <f>IF(C74&gt;C75,C74-C75,0)</f>
+        <v>12.429999999999836</v>
+      </c>
+      <c r="J75" s="42">
+        <f t="shared" si="3"/>
+        <v>3.3567392138195018</v>
+      </c>
+      <c r="K75" s="42">
+        <f t="shared" si="4"/>
+        <v>1.8653144036854743</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="22">
+        <v>41540</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="31">
+        <v>1701.84</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="37">
+        <f t="shared" si="0"/>
+        <v>57.657226854755351</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="42">
+        <f>IF(C76&gt;C75,C76-C75,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H76" s="42">
+        <f t="shared" si="2"/>
+        <v>5.4265241376262559</v>
+      </c>
+      <c r="I76" s="42">
+        <f>IF(C75&gt;C76,C75-C76,0)</f>
+        <v>8.0700000000001637</v>
+      </c>
+      <c r="J76" s="42">
+        <f t="shared" si="3"/>
+        <v>3.985173985310257</v>
+      </c>
+      <c r="K76" s="42">
+        <f t="shared" si="4"/>
+        <v>1.3616780992822288</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="22">
+        <v>41541</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="31">
+        <v>1697.42</v>
+      </c>
+      <c r="D77" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="37">
+        <f t="shared" si="0"/>
+        <v>53.772160755510612</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="42">
+        <f>IF(C77&gt;C76,C77-C76,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H77" s="42">
+        <f t="shared" si="2"/>
+        <v>4.702987585942755</v>
+      </c>
+      <c r="I77" s="42">
+        <f>IF(C76&gt;C77,C76-C77,0)</f>
+        <v>4.4199999999998454</v>
+      </c>
+      <c r="J77" s="42">
+        <f t="shared" si="3"/>
+        <v>4.0431507872688686</v>
+      </c>
+      <c r="K77" s="42">
+        <f t="shared" si="4"/>
+        <v>1.163198661982034</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="22">
+        <v>41542</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="31">
+        <v>1692.77</v>
+      </c>
+      <c r="D78" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="37">
+        <f t="shared" si="0"/>
+        <v>49.706454147087669</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="42">
+        <f>IF(C78&gt;C77,C78-C77,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H78" s="42">
+        <f t="shared" si="2"/>
+        <v>4.0759225744837213</v>
+      </c>
+      <c r="I78" s="42">
+        <f>IF(C77&gt;C78,C77-C78,0)</f>
+        <v>4.6500000000000909</v>
+      </c>
+      <c r="J78" s="42">
+        <f t="shared" si="3"/>
+        <v>4.1240640156330315</v>
+      </c>
+      <c r="K78" s="42">
+        <f t="shared" si="4"/>
+        <v>0.98832669886625879</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="22">
+        <v>41543</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="31">
+        <v>1698.67</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="37">
+        <f t="shared" si="0"/>
+        <v>54.718825049650043</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="42">
+        <f>IF(C79&gt;C78,C79-C78,0)</f>
+        <v>5.9000000000000909</v>
+      </c>
+      <c r="H79" s="42">
+        <f t="shared" si="2"/>
+        <v>4.319132897885904</v>
+      </c>
+      <c r="I79" s="42">
+        <f>IF(C78&gt;C79,C78-C79,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J79" s="42">
+        <f t="shared" si="3"/>
+        <v>3.5741888135486275</v>
+      </c>
+      <c r="K79" s="42">
+        <f t="shared" si="4"/>
+        <v>1.2084232599893512</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="22">
+        <v>41544</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="31">
+        <v>1691.75</v>
+      </c>
+      <c r="D80" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" s="37">
+        <f t="shared" ref="E80:E111" si="5">100-(100 / (1 + K80))</f>
+        <v>48.215709170255948</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="42">
+        <f>IF(C80&gt;C79,C80-C79,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H80" s="42">
+        <f t="shared" si="2"/>
+        <v>3.7432485115011169</v>
+      </c>
+      <c r="I80" s="42">
+        <f>IF(C79&gt;C80,C79-C80,0)</f>
+        <v>6.9200000000000728</v>
+      </c>
+      <c r="J80" s="42">
+        <f t="shared" si="3"/>
+        <v>4.0202969717421535</v>
+      </c>
+      <c r="K80" s="42">
+        <f t="shared" si="4"/>
+        <v>0.93108756338440823</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="22">
+        <v>41547</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="31">
+        <v>1681.55</v>
+      </c>
+      <c r="D81" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="37">
+        <f t="shared" si="5"/>
+        <v>40.108628024901066</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" s="42">
+        <f>IF(C81&gt;C80,C81-C80,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H81" s="42">
+        <f t="shared" ref="H81:H111" si="6">G81*2/(14+1)+H80*(1-2/(14+1))</f>
+        <v>3.2441487099676349</v>
+      </c>
+      <c r="I81" s="42">
+        <f>IF(C80&gt;C81,C80-C81,0)</f>
+        <v>10.200000000000045</v>
+      </c>
+      <c r="J81" s="42">
+        <f t="shared" ref="J81:J111" si="7">I81*2/(14+1)+J80*(1-2/(14+1))</f>
+        <v>4.8442573755098728</v>
+      </c>
+      <c r="K81" s="42">
+        <f t="shared" si="4"/>
+        <v>0.66968958469639084</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="22">
+        <v>41548</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="31">
+        <v>1695</v>
+      </c>
+      <c r="D82" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="37">
+        <f t="shared" si="5"/>
+        <v>52.30920887603444</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="42">
+        <f>IF(C82&gt;C81,C82-C81,0)</f>
+        <v>13.450000000000045</v>
+      </c>
+      <c r="H82" s="42">
+        <f t="shared" si="6"/>
+        <v>4.604928881971956</v>
+      </c>
+      <c r="I82" s="42">
+        <f>IF(C81&gt;C82,C81-C82,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J82" s="42">
+        <f t="shared" si="7"/>
+        <v>4.1983563921085567</v>
+      </c>
+      <c r="K82" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0968408710198148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="22">
+        <v>41549</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="31">
+        <v>1693.87</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="37">
+        <f t="shared" si="5"/>
+        <v>51.296217716570617</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="42">
+        <f>IF(C83&gt;C82,C83-C82,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H83" s="42">
+        <f t="shared" si="6"/>
+        <v>3.9909383643756953</v>
+      </c>
+      <c r="I83" s="42">
+        <f>IF(C82&gt;C83,C82-C83,0)</f>
+        <v>1.1300000000001091</v>
+      </c>
+      <c r="J83" s="42">
+        <f t="shared" si="7"/>
+        <v>3.7892422064940972</v>
+      </c>
+      <c r="K83" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0532286264351025</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="22">
+        <v>41550</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="31">
+        <v>1678.66</v>
+      </c>
+      <c r="D84" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="37">
+        <f t="shared" si="5"/>
+        <v>39.435446200074075</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" s="42">
+        <f>IF(C84&gt;C83,C84-C83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H84" s="42">
+        <f t="shared" si="6"/>
+        <v>3.4588132491256025</v>
+      </c>
+      <c r="I84" s="42">
+        <f>IF(C83&gt;C84,C83-C84,0)</f>
+        <v>15.209999999999809</v>
+      </c>
+      <c r="J84" s="42">
+        <f t="shared" si="7"/>
+        <v>5.312009912294859</v>
+      </c>
+      <c r="K84" s="42">
+        <f t="shared" si="4"/>
+        <v>0.65113079723741496</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="22">
+        <v>41551</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="31">
+        <v>1690.5</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="37">
+        <f t="shared" si="5"/>
+        <v>49.85056117437405</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G85" s="42">
+        <f>IF(C85&gt;C84,C85-C84,0)</f>
+        <v>11.839999999999918</v>
+      </c>
+      <c r="H85" s="42">
+        <f t="shared" si="6"/>
+        <v>4.5763048159088449</v>
+      </c>
+      <c r="I85" s="42">
+        <f>IF(C84&gt;C85,C84-C85,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J85" s="42">
+        <f t="shared" si="7"/>
+        <v>4.6037419239888777</v>
+      </c>
+      <c r="K85" s="42">
+        <f t="shared" si="4"/>
+        <v>0.99404025930796303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="22">
+        <v>41554</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="31">
+        <v>1676.12</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E86" s="37">
+        <f t="shared" si="5"/>
+        <v>40.169965244163528</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G86" s="42">
+        <f>IF(C86&gt;C85,C86-C85,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H86" s="42">
+        <f t="shared" si="6"/>
+        <v>3.9661308404543325</v>
+      </c>
+      <c r="I86" s="42">
+        <f>IF(C85&gt;C86,C85-C86,0)</f>
+        <v>14.380000000000109</v>
+      </c>
+      <c r="J86" s="42">
+        <f t="shared" si="7"/>
+        <v>5.9072430007903751</v>
+      </c>
+      <c r="K86" s="42">
+        <f t="shared" si="4"/>
+        <v>0.67140133560167981</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="22">
+        <v>41555</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="31">
+        <v>1655.45</v>
+      </c>
+      <c r="D87" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="37">
+        <f t="shared" si="5"/>
+        <v>30.383951985827352</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G87" s="42">
+        <f>IF(C87&gt;C86,C87-C86,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H87" s="42">
+        <f t="shared" si="6"/>
+        <v>3.4373133950604218</v>
+      </c>
+      <c r="I87" s="42">
+        <f>IF(C86&gt;C87,C86-C87,0)</f>
+        <v>20.669999999999845</v>
+      </c>
+      <c r="J87" s="42">
+        <f t="shared" si="7"/>
+        <v>7.875610600684972</v>
+      </c>
+      <c r="K87" s="42">
+        <f t="shared" si="4"/>
+        <v>0.43645039976474531</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="22">
+        <v>41556</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="31">
+        <v>1656.4</v>
+      </c>
+      <c r="D88" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" s="37">
+        <f t="shared" si="5"/>
+        <v>31.271864024796116</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" s="42">
+        <f>IF(C88&gt;C87,C88-C87,0)</f>
+        <v>0.95000000000004547</v>
+      </c>
+      <c r="H88" s="42">
+        <f t="shared" si="6"/>
+        <v>3.1056716090523717</v>
+      </c>
+      <c r="I88" s="42">
+        <f>IF(C87&gt;C88,C87-C88,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J88" s="42">
+        <f t="shared" si="7"/>
+        <v>6.825529187260309</v>
+      </c>
+      <c r="K88" s="42">
+        <f t="shared" si="4"/>
+        <v>0.45500817941692129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="22">
+        <v>41557</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="31">
+        <v>1692.56</v>
+      </c>
+      <c r="D89" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="37">
+        <f t="shared" si="5"/>
+        <v>55.948064757359916</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G89" s="42">
+        <f>IF(C89&gt;C88,C89-C88,0)</f>
+        <v>36.159999999999854</v>
+      </c>
+      <c r="H89" s="42">
+        <f t="shared" si="6"/>
+        <v>7.5129153945120368</v>
+      </c>
+      <c r="I89" s="42">
+        <f>IF(C88&gt;C89,C88-C89,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J89" s="42">
+        <f t="shared" si="7"/>
+        <v>5.9154586289589348</v>
+      </c>
+      <c r="K89" s="42">
+        <f t="shared" si="4"/>
+        <v>1.2700478298897746</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="22">
+        <v>41558</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="31">
+        <v>1703.2</v>
+      </c>
+      <c r="D90" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="37">
+        <f t="shared" si="5"/>
+        <v>60.734537198047001</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G90" s="42">
+        <f>IF(C90&gt;C89,C90-C89,0)</f>
+        <v>10.6400000000001</v>
+      </c>
+      <c r="H90" s="42">
+        <f t="shared" si="6"/>
+        <v>7.929860008577112</v>
+      </c>
+      <c r="I90" s="42">
+        <f>IF(C89&gt;C90,C89-C90,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J90" s="42">
+        <f t="shared" si="7"/>
+        <v>5.1267308117644106</v>
+      </c>
+      <c r="K90" s="42">
+        <f t="shared" si="4"/>
+        <v>1.5467673844665895</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="22">
+        <v>41561</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="31">
+        <v>1710.14</v>
+      </c>
+      <c r="D91" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" s="37">
+        <f t="shared" si="5"/>
+        <v>63.702718465131234</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" s="42">
+        <f>IF(C91&gt;C90,C91-C90,0)</f>
+        <v>6.9400000000000546</v>
+      </c>
+      <c r="H91" s="42">
+        <f t="shared" si="6"/>
+        <v>7.7978786741001711</v>
+      </c>
+      <c r="I91" s="42">
+        <f>IF(C90&gt;C91,C90-C91,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J91" s="42">
+        <f t="shared" si="7"/>
+        <v>4.4431667035291564</v>
+      </c>
+      <c r="K91" s="42">
+        <f t="shared" si="4"/>
+        <v>1.7550272574527543</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="22">
+        <v>41562</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="31">
+        <v>1698.06</v>
+      </c>
+      <c r="D92" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="37">
+        <f t="shared" si="5"/>
+        <v>55.306038150886948</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G92" s="42">
+        <f>IF(C92&gt;C91,C92-C91,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H92" s="42">
+        <f t="shared" si="6"/>
+        <v>6.7581615175534822</v>
+      </c>
+      <c r="I92" s="42">
+        <f>IF(C91&gt;C92,C91-C92,0)</f>
+        <v>12.080000000000155</v>
+      </c>
+      <c r="J92" s="42">
+        <f t="shared" si="7"/>
+        <v>5.4614111430586227</v>
+      </c>
+      <c r="K92" s="42">
+        <f t="shared" si="4"/>
+        <v>1.2374387022927236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="22">
+        <v>41563</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="31">
+        <v>1721.54</v>
+      </c>
+      <c r="D93" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E93" s="37">
+        <f t="shared" si="5"/>
+        <v>65.503711363941676</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G93" s="42">
+        <f>IF(C93&gt;C92,C93-C92,0)</f>
+        <v>23.480000000000018</v>
+      </c>
+      <c r="H93" s="42">
+        <f t="shared" si="6"/>
+        <v>8.9877399818796881</v>
+      </c>
+      <c r="I93" s="42">
+        <f>IF(C92&gt;C93,C92-C93,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J93" s="42">
+        <f t="shared" si="7"/>
+        <v>4.7332229906508063</v>
+      </c>
+      <c r="K93" s="42">
+        <f t="shared" si="4"/>
+        <v>1.8988625720006267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="22">
+        <v>41564</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="31">
+        <v>1733.15</v>
+      </c>
+      <c r="D94" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="37">
+        <f t="shared" si="5"/>
+        <v>69.477092060415785</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="42">
+        <f>IF(C94&gt;C93,C94-C93,0)</f>
+        <v>11.610000000000127</v>
+      </c>
+      <c r="H94" s="42">
+        <f t="shared" si="6"/>
+        <v>9.3373746509624134</v>
+      </c>
+      <c r="I94" s="42">
+        <f>IF(C93&gt;C94,C93-C94,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J94" s="42">
+        <f t="shared" si="7"/>
+        <v>4.1021265918973659</v>
+      </c>
+      <c r="K94" s="42">
+        <f t="shared" si="4"/>
+        <v>2.2762278154472009</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="22">
+        <v>41565</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="31">
+        <v>1744.5</v>
+      </c>
+      <c r="D95" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" s="37">
+        <f t="shared" si="5"/>
+        <v>72.986831533760181</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="42">
+        <f>IF(C95&gt;C94,C95-C94,0)</f>
+        <v>11.349999999999909</v>
+      </c>
+      <c r="H95" s="42">
+        <f t="shared" si="6"/>
+        <v>9.6057246975007455</v>
+      </c>
+      <c r="I95" s="42">
+        <f>IF(C94&gt;C95,C94-C95,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J95" s="42">
+        <f t="shared" si="7"/>
+        <v>3.5551763796443838</v>
+      </c>
+      <c r="K95" s="42">
+        <f t="shared" si="4"/>
+        <v>2.7018982103109002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="22">
+        <v>41568</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="31">
+        <v>1744.66</v>
+      </c>
+      <c r="D96" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="37">
+        <f t="shared" si="5"/>
+        <v>73.037261073885162</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G96" s="42">
+        <f>IF(C96&gt;C95,C96-C95,0)</f>
+        <v>0.16000000000008185</v>
+      </c>
+      <c r="H96" s="42">
+        <f t="shared" si="6"/>
+        <v>8.3462947378339898</v>
+      </c>
+      <c r="I96" s="42">
+        <f>IF(C95&gt;C96,C95-C96,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J96" s="42">
+        <f t="shared" si="7"/>
+        <v>3.0811528623584663</v>
+      </c>
+      <c r="K96" s="42">
+        <f t="shared" si="4"/>
+        <v>2.7088220256119731</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="22">
+        <v>41569</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="31">
+        <v>1754.67</v>
+      </c>
+      <c r="D97" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="37">
+        <f t="shared" si="5"/>
+        <v>76.239326678962357</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G97" s="42">
+        <f>IF(C97&gt;C96,C97-C96,0)</f>
+        <v>10.009999999999991</v>
+      </c>
+      <c r="H97" s="42">
+        <f t="shared" si="6"/>
+        <v>8.5681221061227912</v>
+      </c>
+      <c r="I97" s="42">
+        <f>IF(C96&gt;C97,C96-C97,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J97" s="42">
+        <f t="shared" si="7"/>
+        <v>2.670332480710671</v>
+      </c>
+      <c r="K97" s="42">
+        <f t="shared" si="4"/>
+        <v>3.2086349426579672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="22">
+        <v>41570</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="31">
+        <v>1746.38</v>
+      </c>
+      <c r="D98" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="37">
+        <f t="shared" si="5"/>
+        <v>68.469172151453691</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="42">
+        <f>IF(C98&gt;C97,C98-C97,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H98" s="42">
+        <f t="shared" si="6"/>
+        <v>7.4257058253064194</v>
+      </c>
+      <c r="I98" s="42">
+        <f>IF(C97&gt;C98,C97-C98,0)</f>
+        <v>8.2899999999999636</v>
+      </c>
+      <c r="J98" s="42">
+        <f t="shared" si="7"/>
+        <v>3.4196214832825769</v>
+      </c>
+      <c r="K98" s="42">
+        <f t="shared" si="4"/>
+        <v>2.1714993491555403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="22">
+        <v>41571</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="31">
+        <v>1752.07</v>
+      </c>
+      <c r="D99" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="37">
+        <f t="shared" si="5"/>
+        <v>70.82411456348423</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G99" s="42">
+        <f>IF(C99&gt;C98,C99-C98,0)</f>
+        <v>5.6899999999998272</v>
+      </c>
+      <c r="H99" s="42">
+        <f t="shared" si="6"/>
+        <v>7.1942783819322074</v>
+      </c>
+      <c r="I99" s="42">
+        <f>IF(C98&gt;C99,C98-C99,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J99" s="42">
+        <f t="shared" si="7"/>
+        <v>2.9636719521782333</v>
+      </c>
+      <c r="K99" s="42">
+        <f t="shared" si="4"/>
+        <v>2.427488095180228</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="22">
+        <v>41572</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="31">
+        <v>1759.77</v>
+      </c>
+      <c r="D100" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="37">
+        <f t="shared" si="5"/>
+        <v>73.871238433422477</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G100" s="42">
+        <f>IF(C100&gt;C99,C100-C99,0)</f>
+        <v>7.7000000000000455</v>
+      </c>
+      <c r="H100" s="42">
+        <f t="shared" si="6"/>
+        <v>7.2617079310079191</v>
+      </c>
+      <c r="I100" s="42">
+        <f>IF(C99&gt;C100,C99-C100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J100" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5685156918878023</v>
+      </c>
+      <c r="K100" s="42">
+        <f t="shared" si="4"/>
+        <v>2.8272001428462072</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="22">
+        <v>41575</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1762.11</v>
+      </c>
+      <c r="D101" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="37">
+        <f t="shared" si="5"/>
+        <v>74.794314757560556</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="42">
+        <f>IF(C101&gt;C100,C101-C100,0)</f>
+        <v>2.3399999999999181</v>
+      </c>
+      <c r="H101" s="42">
+        <f t="shared" si="6"/>
+        <v>6.6054802068735192</v>
+      </c>
+      <c r="I101" s="42">
+        <f>IF(C100&gt;C101,C100-C101,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J101" s="42">
+        <f t="shared" si="7"/>
+        <v>2.2260469329694286</v>
+      </c>
+      <c r="K101" s="42">
+        <f t="shared" si="4"/>
+        <v>2.9673589128069997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="22">
+        <v>41576</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="31">
+        <v>1771.95</v>
+      </c>
+      <c r="D102" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="37">
+        <f t="shared" si="5"/>
+        <v>78.482681390265924</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G102" s="42">
+        <f>IF(C102&gt;C101,C102-C101,0)</f>
+        <v>9.8400000000001455</v>
+      </c>
+      <c r="H102" s="42">
+        <f t="shared" si="6"/>
+        <v>7.0367495126237358</v>
+      </c>
+      <c r="I102" s="42">
+        <f>IF(C101&gt;C102,C101-C102,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J102" s="42">
+        <f t="shared" si="7"/>
+        <v>1.9292406752401714</v>
+      </c>
+      <c r="K102" s="42">
+        <f t="shared" si="4"/>
+        <v>3.6474192167588058</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="22">
+        <v>41577</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="31">
+        <v>1763.31</v>
+      </c>
+      <c r="D103" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="37">
+        <f t="shared" si="5"/>
+        <v>68.349669637488802</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G103" s="42">
+        <f>IF(C103&gt;C102,C103-C102,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H103" s="42">
+        <f t="shared" si="6"/>
+        <v>6.0985162442739043</v>
+      </c>
+      <c r="I103" s="42">
+        <f>IF(C102&gt;C103,C102-C103,0)</f>
+        <v>8.6400000000001</v>
+      </c>
+      <c r="J103" s="42">
+        <f t="shared" si="7"/>
+        <v>2.824008585208162</v>
+      </c>
+      <c r="K103" s="42">
+        <f t="shared" si="4"/>
+        <v>2.1595246828275392</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="22">
+        <v>41578</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="31">
+        <v>1756.54</v>
+      </c>
+      <c r="D104" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="37">
+        <f t="shared" si="5"/>
+        <v>61.205113477849963</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G104" s="42">
+        <f>IF(C104&gt;C103,C104-C103,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H104" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2853807450373838</v>
+      </c>
+      <c r="I104" s="42">
+        <f>IF(C103&gt;C104,C103-C104,0)</f>
+        <v>6.7699999999999818</v>
+      </c>
+      <c r="J104" s="42">
+        <f t="shared" si="7"/>
+        <v>3.3501407738470714</v>
+      </c>
+      <c r="K104" s="42">
+        <f t="shared" si="4"/>
+        <v>1.5776592990652198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="22">
+        <v>41579</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1761.64</v>
+      </c>
+      <c r="D105" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" s="37">
+        <f t="shared" si="5"/>
+        <v>64.436389745011084</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" s="42">
+        <f>IF(C105&gt;C104,C105-C104,0)</f>
+        <v>5.1000000000001364</v>
+      </c>
+      <c r="H105" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2606633123657511</v>
+      </c>
+      <c r="I105" s="42">
+        <f>IF(C104&gt;C105,C104-C105,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J105" s="42">
+        <f t="shared" si="7"/>
+        <v>2.9034553373341287</v>
+      </c>
+      <c r="K105" s="42">
+        <f t="shared" si="4"/>
+        <v>1.811863004993197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="22">
+        <v>41582</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="31">
+        <v>1767.93</v>
+      </c>
+      <c r="D106" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E106" s="37">
+        <f t="shared" si="5"/>
+        <v>68.20504332731737</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G106" s="42">
+        <f>IF(C106&gt;C105,C106-C105,0)</f>
+        <v>6.2899999999999636</v>
+      </c>
+      <c r="H106" s="42">
+        <f t="shared" si="6"/>
+        <v>5.3979082040503137</v>
+      </c>
+      <c r="I106" s="42">
+        <f>IF(C105&gt;C106,C105-C106,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J106" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5163279590229117</v>
+      </c>
+      <c r="K106" s="42">
+        <f t="shared" si="4"/>
+        <v>2.1451528941983846</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="22">
+        <v>41583</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="31">
+        <v>1762.97</v>
+      </c>
+      <c r="D107" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="37">
+        <f t="shared" si="5"/>
+        <v>62.207138897245812</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G107" s="42">
+        <f>IF(C107&gt;C106,C107-C106,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H107" s="42">
+        <f t="shared" si="6"/>
+        <v>4.678187110176939</v>
+      </c>
+      <c r="I107" s="42">
+        <f>IF(C106&gt;C107,C106-C107,0)</f>
+        <v>4.9600000000000364</v>
+      </c>
+      <c r="J107" s="42">
+        <f t="shared" si="7"/>
+        <v>2.8421508978198617</v>
+      </c>
+      <c r="K107" s="42">
+        <f t="shared" si="4"/>
+        <v>1.6460023687572154</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="22">
+        <v>41584</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="31">
+        <v>1770.49</v>
+      </c>
+      <c r="D108" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E108" s="37">
+        <f t="shared" si="5"/>
+        <v>67.245990756700778</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G108" s="42">
+        <f>IF(C108&gt;C107,C108-C107,0)</f>
+        <v>7.5199999999999818</v>
+      </c>
+      <c r="H108" s="42">
+        <f t="shared" si="6"/>
+        <v>5.0570954954866778</v>
+      </c>
+      <c r="I108" s="42">
+        <f>IF(C107&gt;C108,C107-C108,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J108" s="42">
+        <f t="shared" si="7"/>
+        <v>2.4631974447772138</v>
+      </c>
+      <c r="K108" s="42">
+        <f t="shared" si="4"/>
+        <v>2.0530613598229319</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="22">
+        <v>41585</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="31">
+        <v>1747.15</v>
+      </c>
+      <c r="D109" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="37">
+        <f t="shared" si="5"/>
+        <v>45.514059930927985</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G109" s="42">
+        <f>IF(C109&gt;C108,C109-C108,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H109" s="42">
+        <f t="shared" si="6"/>
+        <v>4.3828160960884546</v>
+      </c>
+      <c r="I109" s="42">
+        <f>IF(C108&gt;C109,C108-C109,0)</f>
+        <v>23.339999999999918</v>
+      </c>
+      <c r="J109" s="42">
+        <f t="shared" si="7"/>
+        <v>5.2467711188069082</v>
+      </c>
+      <c r="K109" s="42">
+        <f t="shared" si="4"/>
+        <v>0.83533586597257303</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="22">
+        <v>41586</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="31">
+        <v>1770.61</v>
+      </c>
+      <c r="D110" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E110" s="37">
+        <f t="shared" si="5"/>
+        <v>60.368281178138361</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" s="42">
+        <f>IF(C110&gt;C109,C110-C109,0)</f>
+        <v>23.459999999999809</v>
+      </c>
+      <c r="H110" s="42">
+        <f t="shared" si="6"/>
+        <v>6.9264406166099679</v>
+      </c>
+      <c r="I110" s="42">
+        <f>IF(C109&gt;C110,C109-C110,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J110" s="42">
+        <f t="shared" si="7"/>
+        <v>4.5472016362993202</v>
+      </c>
+      <c r="K110" s="42">
+        <f t="shared" si="4"/>
+        <v>1.5232314664293092</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="22">
+        <v>41589</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1771.89</v>
+      </c>
+      <c r="D111" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E111" s="37">
+        <f t="shared" si="5"/>
+        <v>61.037006282157336</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="42">
+        <f>IF(C111&gt;C110,C111-C110,0)</f>
+        <v>1.2800000000002001</v>
+      </c>
+      <c r="H111" s="42">
+        <f t="shared" si="6"/>
+        <v>6.1735818677286654</v>
+      </c>
+      <c r="I111" s="42">
+        <f>IF(C110&gt;C111,C110-C111,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J111" s="42">
+        <f t="shared" si="7"/>
+        <v>3.9409080847927442</v>
+      </c>
+      <c r="K111" s="42">
+        <f t="shared" si="4"/>
+        <v>1.5665378980929314</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="22"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="31">
+        <f>COUNT(C2:C111)</f>
+        <v>110</v>
+      </c>
+      <c r="E112" s="37">
+        <f>COUNTIF(E2:E111, "&gt;0")</f>
+        <v>96</v>
+      </c>
+      <c r="F112"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Intraday Trend Strategy now uses RSI to detect divergence (https://app.asana.com/0/186349222941752/239006641226450). Add bonds side control to the strategy. Improved strategy work with algo-orders and added trailing stop. Fix RSI - uses exponential smoothing instead EMA. RelativeStrengthIndexService renamed to Rsi in Indicator namespace.
</commit_message>
<xml_diff>
--- a/sources/Services/Indicators.xlsx
+++ b/sources/Services/Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12660" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MA for S&amp;P 500 (^GSPC)" sheetId="1" r:id="rId1"/>
@@ -9312,9 +9312,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9933,7 +9933,7 @@
       </c>
       <c r="E17" s="34">
         <f t="shared" si="2"/>
-        <v>46.311586248588142</v>
+        <v>44.152272268429215</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>6</v>
@@ -9943,20 +9943,20 @@
         <v>8.6800000000000637</v>
       </c>
       <c r="H17" s="38">
-        <f t="shared" ref="H17:H80" si="4">G17*2/(14+1)+H16*(1-2/(14+1))</f>
-        <v>6.9311904761904835</v>
+        <f>((H16*13)+G17)/14</f>
+        <v>6.8062755102040855</v>
       </c>
       <c r="I17" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J17" s="38">
-        <f t="shared" ref="J17:J80" si="5">I17*2/(14+1)+J16*(1-2/(14+1))</f>
-        <v>8.0352380952380926</v>
+        <f>((J16*13)+I17)/14</f>
+        <v>8.609183673469385</v>
       </c>
       <c r="K17" s="38">
         <f t="shared" si="3"/>
-        <v>0.8625992651416392</v>
+        <v>0.79058314566789212</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="E18" s="34">
         <f t="shared" si="2"/>
-        <v>45.896412506564097</v>
+        <v>43.959238621411288</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>6</v>
@@ -9984,20 +9984,20 @@
         <v>0</v>
       </c>
       <c r="H18" s="38">
-        <f t="shared" si="4"/>
-        <v>6.0070317460317524</v>
+        <f t="shared" ref="H18:H81" si="4">((H17*13)+G18)/14</f>
+        <v>6.3201129737609367</v>
       </c>
       <c r="I18" s="38">
         <f t="shared" si="1"/>
         <v>0.88000000000010914</v>
       </c>
       <c r="J18" s="38">
-        <f t="shared" si="5"/>
-        <v>7.0812063492063615</v>
+        <f t="shared" ref="J18:J81" si="5">((J17*13)+I18)/14</f>
+        <v>8.0570991253644362</v>
       </c>
       <c r="K18" s="38">
         <f t="shared" si="3"/>
-        <v>0.84830627011808535</v>
+        <v>0.78441544226068671</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -10015,7 +10015,7 @@
       </c>
       <c r="E19" s="34">
         <f t="shared" si="2"/>
-        <v>46.729222887030637</v>
+        <v>44.355204858855309</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>6</v>
@@ -10026,7 +10026,7 @@
       </c>
       <c r="H19" s="38">
         <f t="shared" si="4"/>
-        <v>5.3834275132275398</v>
+        <v>5.9636763327780233</v>
       </c>
       <c r="I19" s="38">
         <f t="shared" si="1"/>
@@ -10034,11 +10034,11 @@
       </c>
       <c r="J19" s="38">
         <f t="shared" si="5"/>
-        <v>6.1370455026455133</v>
+        <v>7.4815920449812623</v>
       </c>
       <c r="K19" s="38">
         <f t="shared" si="3"/>
-        <v>0.87720182470651242</v>
+        <v>0.7971132744104279</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -10056,7 +10056,7 @@
       </c>
       <c r="E20" s="34">
         <f t="shared" si="2"/>
-        <v>56.338164033492767</v>
+        <v>49.14964972088061</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>6</v>
@@ -10067,7 +10067,7 @@
       </c>
       <c r="H20" s="38">
         <f t="shared" si="4"/>
-        <v>6.8629705114638702</v>
+        <v>6.7148423090081666</v>
       </c>
       <c r="I20" s="38">
         <f t="shared" si="1"/>
@@ -10075,11 +10075,11 @@
       </c>
       <c r="J20" s="38">
         <f t="shared" si="5"/>
-        <v>5.3187727689594446</v>
+        <v>6.9471926131968855</v>
       </c>
       <c r="K20" s="38">
         <f t="shared" si="3"/>
-        <v>1.2903297075438944</v>
+        <v>0.96655479167982961</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -10097,7 +10097,7 @@
       </c>
       <c r="E21" s="34">
         <f t="shared" si="2"/>
-        <v>60.602280925995679</v>
+        <v>51.490372688558253</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>6</v>
@@ -10108,7 +10108,7 @@
       </c>
       <c r="H21" s="38">
         <f t="shared" si="4"/>
-        <v>7.0905744432686788</v>
+        <v>6.8473535726504355</v>
       </c>
       <c r="I21" s="38">
         <f t="shared" si="1"/>
@@ -10116,11 +10116,11 @@
       </c>
       <c r="J21" s="38">
         <f t="shared" si="5"/>
-        <v>4.6096030664315188</v>
+        <v>6.4509645693971081</v>
       </c>
       <c r="K21" s="38">
         <f t="shared" si="3"/>
-        <v>1.5382180072953182</v>
+        <v>1.0614464703672017</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="E22" s="34">
         <f t="shared" si="2"/>
-        <v>65.917385186956011</v>
+        <v>54.604641311423251</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>6</v>
@@ -10149,7 +10149,7 @@
       </c>
       <c r="H22" s="38">
         <f t="shared" si="4"/>
-        <v>7.7264978508328417</v>
+        <v>7.2053997460325405</v>
       </c>
       <c r="I22" s="38">
         <f t="shared" si="1"/>
@@ -10157,11 +10157,11 @@
       </c>
       <c r="J22" s="38">
         <f t="shared" si="5"/>
-        <v>3.9949893242406498</v>
+        <v>5.9901813858687438</v>
       </c>
       <c r="K22" s="38">
         <f t="shared" si="3"/>
-        <v>1.9340471835432154</v>
+        <v>1.2028683744085917</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -10179,7 +10179,7 @@
       </c>
       <c r="E23" s="34">
         <f t="shared" si="2"/>
-        <v>66.051060556366423</v>
+        <v>54.683891806908377</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>6</v>
@@ -10190,7 +10190,7 @@
       </c>
       <c r="H23" s="38">
         <f t="shared" si="4"/>
-        <v>6.7362981373884567</v>
+        <v>6.7121569070302129</v>
       </c>
       <c r="I23" s="38">
         <f t="shared" si="1"/>
@@ -10198,11 +10198,11 @@
       </c>
       <c r="J23" s="38">
         <f t="shared" si="5"/>
-        <v>3.4623240810085631</v>
+        <v>5.5623112868781197</v>
       </c>
       <c r="K23" s="38">
         <f t="shared" si="3"/>
-        <v>1.945600117082684</v>
+        <v>1.2067208325547438</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -10220,7 +10220,7 @@
       </c>
       <c r="E24" s="34">
         <f t="shared" si="2"/>
-        <v>74.625277361614764</v>
+        <v>60.262237125218796</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>6</v>
@@ -10231,7 +10231,7 @@
       </c>
       <c r="H24" s="38">
         <f t="shared" si="4"/>
-        <v>8.8247917190700083</v>
+        <v>7.8327171279566334</v>
       </c>
       <c r="I24" s="38">
         <f t="shared" si="1"/>
@@ -10239,11 +10239,11 @@
       </c>
       <c r="J24" s="38">
         <f t="shared" si="5"/>
-        <v>3.0006808702074217</v>
+        <v>5.1650033378153974</v>
       </c>
       <c r="K24" s="38">
         <f t="shared" si="3"/>
-        <v>2.9409297758678337</v>
+        <v>1.5164979798966749</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -10261,7 +10261,7 @@
       </c>
       <c r="E25" s="34">
         <f t="shared" si="2"/>
-        <v>76.224428962725369</v>
+        <v>61.441999398129667</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>6</v>
@@ -10272,7 +10272,7 @@
       </c>
       <c r="H25" s="38">
         <f t="shared" si="4"/>
-        <v>8.3374861565273513</v>
+        <v>7.6425230473883081</v>
       </c>
       <c r="I25" s="38">
         <f t="shared" si="1"/>
@@ -10280,11 +10280,11 @@
       </c>
       <c r="J25" s="38">
         <f t="shared" si="5"/>
-        <v>2.6005900875130989</v>
+        <v>4.7960745279714407</v>
       </c>
       <c r="K25" s="38">
         <f t="shared" si="3"/>
-        <v>3.2059978220175216</v>
+        <v>1.593495472769646</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -10302,7 +10302,7 @@
       </c>
       <c r="E26" s="34">
         <f t="shared" si="2"/>
-        <v>76.972602819597554</v>
+        <v>61.985063973409545</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>6</v>
@@ -10313,7 +10313,7 @@
       </c>
       <c r="H26" s="38">
         <f t="shared" si="4"/>
-        <v>7.5338213356570307</v>
+        <v>7.2616285440034245</v>
       </c>
       <c r="I26" s="38">
         <f t="shared" si="1"/>
@@ -10321,11 +10321,11 @@
       </c>
       <c r="J26" s="38">
         <f t="shared" si="5"/>
-        <v>2.2538447425113524</v>
+        <v>4.4534977759734806</v>
       </c>
       <c r="K26" s="38">
         <f t="shared" si="3"/>
-        <v>3.3426531976920693</v>
+        <v>1.6305450028918271</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -10340,7 +10340,7 @@
       </c>
       <c r="E27" s="34">
         <f t="shared" si="2"/>
-        <v>2.80449473479527</v>
+        <v>5.1450481706205267</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>6</v>
@@ -10351,7 +10351,7 @@
       </c>
       <c r="H27" s="38">
         <f t="shared" si="4"/>
-        <v>6.5293118242360935</v>
+        <v>6.7429407908603229</v>
       </c>
       <c r="I27" s="38">
         <f t="shared" si="1"/>
@@ -10359,11 +10359,11 @@
       </c>
       <c r="J27" s="38">
         <f t="shared" si="5"/>
-        <v>226.28666544350986</v>
+        <v>124.31396222054681</v>
       </c>
       <c r="K27" s="38">
         <f t="shared" si="3"/>
-        <v>2.8854160767445083E-2</v>
+        <v>5.4241218527791714E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="E28" s="34">
         <f t="shared" si="2"/>
-        <v>53.885126822286999</v>
+        <v>52.186933917505684</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>6</v>
@@ -10392,7 +10392,7 @@
       </c>
       <c r="H28" s="38">
         <f t="shared" si="4"/>
-        <v>229.16007024767126</v>
+        <v>125.99415930579887</v>
       </c>
       <c r="I28" s="38">
         <f t="shared" si="1"/>
@@ -10400,11 +10400,11 @@
       </c>
       <c r="J28" s="38">
         <f t="shared" si="5"/>
-        <v>196.11511005104188</v>
+        <v>115.43439349050776</v>
       </c>
       <c r="K28" s="38">
         <f t="shared" si="3"/>
-        <v>1.1684977775961727</v>
+        <v>1.0914785056341068</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -10422,7 +10422,7 @@
       </c>
       <c r="E29" s="34">
         <f t="shared" si="2"/>
-        <v>53.962569548790583</v>
+        <v>52.257667328901917</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>6</v>
@@ -10433,7 +10433,7 @@
       </c>
       <c r="H29" s="38">
         <f t="shared" si="4"/>
-        <v>199.22539421464845</v>
+        <v>117.32671935538467</v>
       </c>
       <c r="I29" s="38">
         <f t="shared" si="1"/>
@@ -10441,11 +10441,11 @@
       </c>
       <c r="J29" s="38">
         <f t="shared" si="5"/>
-        <v>169.96642871090296</v>
+        <v>107.18907966975721</v>
       </c>
       <c r="K29" s="38">
         <f t="shared" si="3"/>
-        <v>1.1721455567764636</v>
+        <v>1.0945771688390356</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="E30" s="34">
         <f t="shared" si="2"/>
-        <v>54.12429845583042</v>
+        <v>52.395650695385477</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>6</v>
@@ -10474,7 +10474,7 @@
       </c>
       <c r="H30" s="38">
         <f t="shared" si="4"/>
-        <v>173.79000831936199</v>
+        <v>109.55052511571432</v>
       </c>
       <c r="I30" s="38">
         <f t="shared" si="1"/>
@@ -10482,11 +10482,11 @@
       </c>
       <c r="J30" s="38">
         <f t="shared" si="5"/>
-        <v>147.30423821611589</v>
+        <v>99.532716836203122</v>
       </c>
       <c r="K30" s="38">
         <f t="shared" si="3"/>
-        <v>1.1798031775867017</v>
+        <v>1.1006483958033326</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -10504,7 +10504,7 @@
       </c>
       <c r="E31" s="34">
         <f t="shared" si="2"/>
-        <v>54.184007500493628</v>
+        <v>52.443241010002303</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>6</v>
@@ -10515,7 +10515,7 @@
       </c>
       <c r="H31" s="38">
         <f t="shared" si="4"/>
-        <v>150.9806738767804</v>
+        <v>101.91977332173472</v>
       </c>
       <c r="I31" s="38">
         <f t="shared" si="1"/>
@@ -10523,11 +10523,11 @@
       </c>
       <c r="J31" s="38">
         <f t="shared" si="5"/>
-        <v>127.66367312063377</v>
+        <v>92.423237062188619</v>
       </c>
       <c r="K31" s="38">
         <f t="shared" si="3"/>
-        <v>1.1826439752686231</v>
+        <v>1.10275052639799</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -10545,7 +10545,7 @@
       </c>
       <c r="E32" s="34">
         <f t="shared" si="2"/>
-        <v>54.270861110163871</v>
+        <v>52.50790574254556</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>6</v>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="H32" s="38">
         <f t="shared" si="4"/>
-        <v>131.30858402654303</v>
+        <v>94.885503798753675</v>
       </c>
       <c r="I32" s="38">
         <f t="shared" si="1"/>
@@ -10564,11 +10564,11 @@
       </c>
       <c r="J32" s="38">
         <f t="shared" si="5"/>
-        <v>110.64185003788261</v>
+        <v>85.821577272032286</v>
       </c>
       <c r="K32" s="38">
         <f t="shared" si="3"/>
-        <v>1.1867894831981241</v>
+        <v>1.1056136092441073</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="E33" s="34">
         <f t="shared" si="2"/>
-        <v>54.162720117233299</v>
+        <v>52.437815797651581</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>6</v>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="H33" s="38">
         <f t="shared" si="4"/>
-        <v>113.80077282300397</v>
+        <v>88.107967813128411</v>
       </c>
       <c r="I33" s="38">
         <f t="shared" si="1"/>
@@ -10605,11 +10605,11 @@
       </c>
       <c r="J33" s="38">
         <f t="shared" si="5"/>
-        <v>96.308270032831587</v>
+        <v>79.915750324029972</v>
       </c>
       <c r="K33" s="38">
         <f t="shared" si="3"/>
-        <v>1.1816303291940471</v>
+        <v>1.102510674752873</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -10627,7 +10627,7 @@
       </c>
       <c r="E34" s="34">
         <f t="shared" si="2"/>
-        <v>53.908121633286683</v>
+        <v>52.283429115026465</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>6</v>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="H34" s="38">
         <f t="shared" si="4"/>
-        <v>98.627336446603437</v>
+        <v>81.814541540762093</v>
       </c>
       <c r="I34" s="38">
         <f t="shared" si="1"/>
@@ -10646,11 +10646,11 @@
       </c>
       <c r="J34" s="38">
         <f t="shared" si="5"/>
-        <v>84.327167361787374</v>
+        <v>74.668196729456412</v>
       </c>
       <c r="K34" s="38">
         <f t="shared" si="3"/>
-        <v>1.1695796210426979</v>
+        <v>1.0957080139111819</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -10668,7 +10668,7 @@
       </c>
       <c r="E35" s="34">
         <f t="shared" si="2"/>
-        <v>54.074567900384231</v>
+        <v>52.384312011857077</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>6</v>
@@ -10679,7 +10679,7 @@
       </c>
       <c r="H35" s="38">
         <f t="shared" si="4"/>
-        <v>86.051691587056311</v>
+        <v>76.278502859279087</v>
       </c>
       <c r="I35" s="38">
         <f t="shared" ref="I35:I66" si="7">IF(C34&gt;C35,C34-C35,0)</f>
@@ -10687,11 +10687,11 @@
       </c>
       <c r="J35" s="38">
         <f t="shared" si="5"/>
-        <v>73.083545046882392</v>
+        <v>69.334754105923807</v>
       </c>
       <c r="K35" s="38">
         <f t="shared" si="3"/>
-        <v>1.1774427681614921</v>
+        <v>1.1001481701766362</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -10709,7 +10709,7 @@
       </c>
       <c r="E36" s="34">
         <f t="shared" si="2"/>
-        <v>54.136642534619092</v>
+        <v>52.419501484251995</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>6</v>
@@ -10720,7 +10720,7 @@
       </c>
       <c r="H36" s="38">
         <f t="shared" si="4"/>
-        <v>74.764799375448817</v>
+        <v>70.930038369330589</v>
       </c>
       <c r="I36" s="38">
         <f t="shared" si="7"/>
@@ -10728,11 +10728,11 @@
       </c>
       <c r="J36" s="38">
         <f t="shared" si="5"/>
-        <v>63.33907237396474</v>
+        <v>64.382271669786391</v>
       </c>
       <c r="K36" s="38">
         <f t="shared" si="3"/>
-        <v>1.1803898695267374</v>
+        <v>1.1017013927860044</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -10750,7 +10750,7 @@
       </c>
       <c r="E37" s="34">
         <f t="shared" si="2"/>
-        <v>53.758163098504149</v>
+        <v>52.231841465641125</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>6</v>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="H37" s="38">
         <f t="shared" si="4"/>
-        <v>64.796159458722315</v>
+        <v>65.863607057235541</v>
       </c>
       <c r="I37" s="38">
         <f t="shared" si="7"/>
@@ -10769,11 +10769,11 @@
       </c>
       <c r="J37" s="38">
         <f t="shared" si="5"/>
-        <v>55.736529390769462</v>
+        <v>60.234966550515942</v>
       </c>
       <c r="K37" s="38">
         <f t="shared" si="3"/>
-        <v>1.1625438499127867</v>
+        <v>1.0934447353266006</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
       </c>
       <c r="E38" s="34">
         <f t="shared" si="2"/>
-        <v>53.795317334876913</v>
+        <v>52.250192419742966</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>6</v>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="H38" s="38">
         <f t="shared" si="4"/>
-        <v>56.240671530892691</v>
+        <v>61.20406369600444</v>
       </c>
       <c r="I38" s="38">
         <f t="shared" si="7"/>
@@ -10810,11 +10810,11 @@
       </c>
       <c r="J38" s="38">
         <f t="shared" si="5"/>
-        <v>48.304992138666869</v>
+        <v>55.932468939764803</v>
       </c>
       <c r="K38" s="38">
         <f t="shared" si="3"/>
-        <v>1.1642828006150014</v>
+        <v>1.0942492769614149</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -10832,7 +10832,7 @@
       </c>
       <c r="E39" s="34">
         <f t="shared" si="2"/>
-        <v>53.77711588590882</v>
+        <v>52.242301739900064</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>6</v>
@@ -10843,7 +10843,7 @@
       </c>
       <c r="H39" s="38">
         <f t="shared" si="4"/>
-        <v>48.741915326773665</v>
+        <v>56.832344860575553</v>
       </c>
       <c r="I39" s="38">
         <f t="shared" si="7"/>
@@ -10851,11 +10851,11 @@
       </c>
       <c r="J39" s="38">
         <f t="shared" si="5"/>
-        <v>41.894993186844623</v>
+        <v>51.953721158353027</v>
       </c>
       <c r="K39" s="38">
         <f t="shared" si="3"/>
-        <v>1.1634305586205236</v>
+        <v>1.0939032583893782</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -10873,7 +10873,7 @@
       </c>
       <c r="E40" s="34">
         <f t="shared" si="2"/>
-        <v>55.37826932652532</v>
+        <v>52.945678275613346</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>6</v>
@@ -10884,7 +10884,7 @@
       </c>
       <c r="H40" s="38">
         <f t="shared" si="4"/>
-        <v>45.061659949870496</v>
+        <v>54.282891656248715</v>
       </c>
       <c r="I40" s="38">
         <f t="shared" si="7"/>
@@ -10892,11 +10892,11 @@
       </c>
       <c r="J40" s="38">
         <f t="shared" si="5"/>
-        <v>36.308994095265341</v>
+        <v>48.242741075613523</v>
       </c>
       <c r="K40" s="38">
         <f t="shared" si="3"/>
-        <v>1.2410605436118787</v>
+        <v>1.1252033040819163</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -10914,7 +10914,7 @@
       </c>
       <c r="E41" s="34">
         <f t="shared" si="2"/>
-        <v>55.613248961695895</v>
+        <v>53.044322198444462</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>6</v>
@@ -10925,7 +10925,7 @@
       </c>
       <c r="H41" s="38">
         <f t="shared" si="4"/>
-        <v>39.426771956554454</v>
+        <v>50.605542252230961</v>
       </c>
       <c r="I41" s="38">
         <f t="shared" si="7"/>
@@ -10933,11 +10933,11 @@
       </c>
       <c r="J41" s="38">
         <f t="shared" si="5"/>
-        <v>31.467794882563297</v>
+        <v>44.796830998783989</v>
       </c>
       <c r="K41" s="38">
         <f t="shared" si="3"/>
-        <v>1.2529245250165695</v>
+        <v>1.1296679056070875</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -10955,7 +10955,7 @@
       </c>
       <c r="E42" s="34">
         <f t="shared" si="2"/>
-        <v>55.309584056078585</v>
+        <v>52.936335102682897</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>6</v>
@@ -10966,7 +10966,7 @@
       </c>
       <c r="H42" s="38">
         <f t="shared" si="4"/>
-        <v>34.16986902901386</v>
+        <v>46.990860662785892</v>
       </c>
       <c r="I42" s="38">
         <f t="shared" si="7"/>
@@ -10974,11 +10974,11 @@
       </c>
       <c r="J42" s="38">
         <f t="shared" si="5"/>
-        <v>27.609422231554856</v>
+        <v>41.777771641727988</v>
       </c>
       <c r="K42" s="38">
         <f t="shared" si="3"/>
-        <v>1.2376162290698376</v>
+        <v>1.1247814044694291</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -10996,7 +10996,7 @@
       </c>
       <c r="E43" s="34">
         <f t="shared" si="2"/>
-        <v>53.995875960034823</v>
+        <v>52.491924736816593</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>6</v>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="H43" s="38">
         <f t="shared" si="4"/>
-        <v>29.613886491812014</v>
+        <v>43.634370615444041</v>
       </c>
       <c r="I43" s="38">
         <f t="shared" si="7"/>
@@ -11015,11 +11015,11 @@
       </c>
       <c r="J43" s="38">
         <f t="shared" si="5"/>
-        <v>25.230832600680905</v>
+        <v>39.491502238747437</v>
       </c>
       <c r="K43" s="38">
         <f t="shared" si="3"/>
-        <v>1.1737181630309268</v>
+        <v>1.1049053123289849</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -11037,7 +11037,7 @@
       </c>
       <c r="E44" s="34">
         <f t="shared" si="2"/>
-        <v>53.034827025312218</v>
+        <v>52.179994856173515</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>6</v>
@@ -11048,7 +11048,7 @@
       </c>
       <c r="H44" s="38">
         <f t="shared" si="4"/>
-        <v>25.665368292903747</v>
+        <v>40.517629857198038</v>
       </c>
       <c r="I44" s="38">
         <f t="shared" si="7"/>
@@ -11056,11 +11056,11 @@
       </c>
       <c r="J44" s="38">
         <f t="shared" si="5"/>
-        <v>22.728054920590093</v>
+        <v>37.13210922169403</v>
       </c>
       <c r="K44" s="38">
         <f t="shared" si="3"/>
-        <v>1.1292373404841012</v>
+        <v>1.0911750155449305</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -11078,7 +11078,7 @@
       </c>
       <c r="E45" s="34">
         <f t="shared" si="2"/>
-        <v>53.995695919467792</v>
+        <v>52.489219559109692</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>6</v>
@@ -11089,7 +11089,7 @@
       </c>
       <c r="H45" s="38">
         <f t="shared" si="4"/>
-        <v>23.119319187183237</v>
+        <v>38.092799153112459</v>
       </c>
       <c r="I45" s="38">
         <f t="shared" si="7"/>
@@ -11097,11 +11097,11 @@
       </c>
       <c r="J45" s="38">
         <f t="shared" si="5"/>
-        <v>19.69764759784475</v>
+        <v>34.479815705858741</v>
       </c>
       <c r="K45" s="38">
         <f t="shared" si="3"/>
-        <v>1.1737096560562326</v>
+        <v>1.1047854628364446</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
       </c>
       <c r="E46" s="34">
         <f t="shared" si="2"/>
-        <v>52.845034491166736</v>
+        <v>52.154218682001869</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>6</v>
@@ -11130,7 +11130,7 @@
       </c>
       <c r="H46" s="38">
         <f t="shared" si="4"/>
-        <v>20.036743295558807</v>
+        <v>35.371884927890143</v>
       </c>
       <c r="I46" s="38">
         <f t="shared" si="7"/>
@@ -11138,11 +11138,11 @@
       </c>
       <c r="J46" s="38">
         <f t="shared" si="5"/>
-        <v>17.879294584798775</v>
+        <v>32.44982886972597</v>
       </c>
       <c r="K46" s="38">
         <f t="shared" si="3"/>
-        <v>1.1206674402352723</v>
+        <v>1.0900484273706079</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -11160,7 +11160,7 @@
       </c>
       <c r="E47" s="34">
         <f t="shared" si="2"/>
-        <v>52.430195297292606</v>
+        <v>52.039124735340565</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>6</v>
@@ -11171,7 +11171,7 @@
       </c>
       <c r="H47" s="38">
         <f t="shared" si="4"/>
-        <v>17.365177522817632</v>
+        <v>32.84532171875513</v>
       </c>
       <c r="I47" s="38">
         <f t="shared" si="7"/>
@@ -11179,11 +11179,11 @@
       </c>
       <c r="J47" s="38">
         <f t="shared" si="5"/>
-        <v>15.755388640158944</v>
+        <v>30.271269664745546</v>
       </c>
       <c r="K47" s="38">
         <f t="shared" si="3"/>
-        <v>1.1021738606025555</v>
+        <v>1.0850328407931753</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -11201,7 +11201,7 @@
       </c>
       <c r="E48" s="34">
         <f t="shared" si="2"/>
-        <v>53.444418380688347</v>
+        <v>52.311707084524762</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>6</v>
@@ -11212,7 +11212,7 @@
       </c>
       <c r="H48" s="38">
         <f t="shared" si="4"/>
-        <v>15.675153853108622</v>
+        <v>30.834227310272627</v>
       </c>
       <c r="I48" s="38">
         <f t="shared" si="7"/>
@@ -11220,11 +11220,11 @@
       </c>
       <c r="J48" s="38">
         <f t="shared" si="5"/>
-        <v>13.654670154804419</v>
+        <v>28.10903611726372</v>
       </c>
       <c r="K48" s="38">
         <f t="shared" si="3"/>
-        <v>1.1479701578579173</v>
+        <v>1.0969507165468111</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
       </c>
       <c r="E49" s="34">
         <f t="shared" si="2"/>
-        <v>51.093992194266569</v>
+        <v>51.719765822979561</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>6</v>
@@ -11253,7 +11253,7 @@
       </c>
       <c r="H49" s="38">
         <f t="shared" si="4"/>
-        <v>13.585133339360807</v>
+        <v>28.631782502396014</v>
       </c>
       <c r="I49" s="38">
         <f t="shared" si="7"/>
@@ -11261,11 +11261,11 @@
       </c>
       <c r="J49" s="38">
         <f t="shared" si="5"/>
-        <v>13.003380800830495</v>
+        <v>26.727676394602025</v>
       </c>
       <c r="K49" s="38">
         <f t="shared" si="3"/>
-        <v>1.0447385604898347</v>
+        <v>1.0712409892907317</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -11283,7 +11283,7 @@
       </c>
       <c r="E50" s="34">
         <f t="shared" si="2"/>
-        <v>44.847869862584453</v>
+        <v>50.045941906873324</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>6</v>
@@ -11294,7 +11294,7 @@
       </c>
       <c r="H50" s="38">
         <f t="shared" si="4"/>
-        <v>11.773782227446032</v>
+        <v>26.586655180796299</v>
       </c>
       <c r="I50" s="38">
         <f t="shared" si="7"/>
@@ -11302,11 +11302,11 @@
       </c>
       <c r="J50" s="38">
         <f t="shared" si="5"/>
-        <v>14.478930027386451</v>
+        <v>26.537842366416179</v>
       </c>
       <c r="K50" s="38">
         <f t="shared" si="3"/>
-        <v>0.81316659485032983</v>
+        <v>1.0018393663548886</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -11324,7 +11324,7 @@
       </c>
       <c r="E51" s="34">
         <f t="shared" si="2"/>
-        <v>43.449975525652732</v>
+        <v>49.651244480173098</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>6</v>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="H51" s="38">
         <f t="shared" si="4"/>
-        <v>10.203944597119895</v>
+        <v>24.687608382167991</v>
       </c>
       <c r="I51" s="38">
         <f t="shared" si="7"/>
@@ -11343,11 +11343,11 @@
       </c>
       <c r="J51" s="38">
         <f t="shared" si="5"/>
-        <v>13.280406023734926</v>
+        <v>25.034425054529311</v>
       </c>
       <c r="K51" s="38">
         <f t="shared" si="3"/>
-        <v>0.76834583060813522</v>
+        <v>0.98614640952984167</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -11365,7 +11365,7 @@
       </c>
       <c r="E52" s="34">
         <f t="shared" si="2"/>
-        <v>40.836314899482119</v>
+        <v>48.911950261699054</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>6</v>
@@ -11376,7 +11376,7 @@
       </c>
       <c r="H52" s="38">
         <f t="shared" si="4"/>
-        <v>8.8434186508372417</v>
+        <v>22.924207783441705</v>
       </c>
       <c r="I52" s="38">
         <f t="shared" si="7"/>
@@ -11384,11 +11384,11 @@
       </c>
       <c r="J52" s="38">
         <f t="shared" si="5"/>
-        <v>12.812351887236932</v>
+        <v>23.94410897920579</v>
       </c>
       <c r="K52" s="38">
         <f t="shared" si="3"/>
-        <v>0.69022602006791922</v>
+        <v>0.95740492174297165</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -11406,7 +11406,7 @@
       </c>
       <c r="E53" s="34">
         <f t="shared" si="2"/>
-        <v>43.366972710658636</v>
+        <v>49.43396984540783</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>6</v>
@@ -11417,7 +11417,7 @@
       </c>
       <c r="H53" s="38">
         <f t="shared" si="4"/>
-        <v>8.502962830725604</v>
+        <v>21.736050084624441</v>
       </c>
       <c r="I53" s="38">
         <f t="shared" si="7"/>
@@ -11425,11 +11425,11 @@
       </c>
       <c r="J53" s="38">
         <f t="shared" si="5"/>
-        <v>11.104038302272009</v>
+        <v>22.233815480691089</v>
       </c>
       <c r="K53" s="38">
         <f t="shared" si="3"/>
-        <v>0.76575409767686087</v>
+        <v>0.97761223679764142</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
       </c>
       <c r="E54" s="34">
         <f t="shared" si="2"/>
-        <v>40.343847373526913</v>
+        <v>48.621636182218182</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>6</v>
@@ -11458,7 +11458,7 @@
       </c>
       <c r="H54" s="38">
         <f t="shared" si="4"/>
-        <v>7.3692344532955234</v>
+        <v>20.183475078579839</v>
       </c>
       <c r="I54" s="38">
         <f t="shared" si="7"/>
@@ -11466,11 +11466,11 @@
       </c>
       <c r="J54" s="38">
         <f t="shared" si="5"/>
-        <v>10.896833195302403</v>
+        <v>21.327828660641721</v>
       </c>
       <c r="K54" s="38">
         <f t="shared" si="3"/>
-        <v>0.6762730346714293</v>
+        <v>0.94634458105087527</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -11488,7 +11488,7 @@
       </c>
       <c r="E55" s="34">
         <f t="shared" si="2"/>
-        <v>46.700493341760897</v>
+        <v>49.935302674641129</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>6</v>
@@ -11499,7 +11499,7 @@
       </c>
       <c r="H55" s="38">
         <f t="shared" si="4"/>
-        <v>8.274669859522799</v>
+        <v>19.753226858681284</v>
       </c>
       <c r="I55" s="38">
         <f t="shared" si="7"/>
@@ -11507,11 +11507,11 @@
       </c>
       <c r="J55" s="38">
         <f t="shared" si="5"/>
-        <v>9.4439221025954154</v>
+        <v>19.804412327738738</v>
       </c>
       <c r="K55" s="38">
         <f t="shared" si="3"/>
-        <v>0.87618997378734431</v>
+        <v>0.99741545125346831</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -11529,7 +11529,7 @@
       </c>
       <c r="E56" s="34">
         <f t="shared" si="2"/>
-        <v>49.564484349777594</v>
+        <v>50.564008207921596</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>6</v>
@@ -11540,7 +11540,7 @@
       </c>
       <c r="H56" s="38">
         <f t="shared" si="4"/>
-        <v>8.0433805449197546</v>
+        <v>18.809424940204046</v>
       </c>
       <c r="I56" s="38">
         <f t="shared" si="7"/>
@@ -11548,11 +11548,11 @@
       </c>
       <c r="J56" s="38">
         <f t="shared" si="5"/>
-        <v>8.1847324889160262</v>
+        <v>18.38981144718597</v>
       </c>
       <c r="K56" s="38">
         <f t="shared" si="3"/>
-        <v>0.98272980281424049</v>
+        <v>1.0228177158979128</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -11570,7 +11570,7 @@
       </c>
       <c r="E57" s="34">
         <f t="shared" si="2"/>
-        <v>46.595988656139781</v>
+        <v>49.870997491145573</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>6</v>
@@ -11581,7 +11581,7 @@
       </c>
       <c r="H57" s="38">
         <f t="shared" si="4"/>
-        <v>6.9709298055971205</v>
+        <v>17.465894587332329</v>
       </c>
       <c r="I57" s="38">
         <f t="shared" si="7"/>
@@ -11589,11 +11589,11 @@
       </c>
       <c r="J57" s="38">
         <f t="shared" si="5"/>
-        <v>7.9894348237272261</v>
+        <v>17.556253486672688</v>
       </c>
       <c r="K57" s="38">
         <f t="shared" si="3"/>
-        <v>0.87251851468825758</v>
+        <v>0.99485317870302159</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="E58" s="34">
         <f t="shared" si="2"/>
-        <v>36.676521344984188</v>
+        <v>47.147492257661071</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>6</v>
@@ -11622,7 +11622,7 @@
       </c>
       <c r="H58" s="38">
         <f t="shared" si="4"/>
-        <v>6.041472498184171</v>
+        <v>16.218330688237163</v>
       </c>
       <c r="I58" s="38">
         <f t="shared" si="7"/>
@@ -11630,11 +11630,11 @@
       </c>
       <c r="J58" s="38">
         <f t="shared" si="5"/>
-        <v>10.430843513896924</v>
+        <v>18.180806809053205</v>
       </c>
       <c r="K58" s="38">
         <f t="shared" si="3"/>
-        <v>0.57919309115654627</v>
+        <v>0.8920578090165493</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -11652,7 +11652,7 @@
       </c>
       <c r="E59" s="34">
         <f t="shared" si="2"/>
-        <v>39.219677300558757</v>
+        <v>47.671724264071628</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>6</v>
@@ -11663,7 +11663,7 @@
       </c>
       <c r="H59" s="38">
         <f t="shared" si="4"/>
-        <v>5.8332761650929505</v>
+        <v>15.379878496220226</v>
       </c>
       <c r="I59" s="38">
         <f t="shared" si="7"/>
@@ -11671,11 +11671,11 @@
       </c>
       <c r="J59" s="38">
         <f t="shared" si="5"/>
-        <v>9.0400643787106674</v>
+        <v>16.88217775126369</v>
       </c>
       <c r="K59" s="38">
         <f t="shared" si="3"/>
-        <v>0.64526931675733457</v>
+        <v>0.91101270954625435</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -11693,7 +11693,7 @@
       </c>
       <c r="E60" s="34">
         <f t="shared" si="2"/>
-        <v>41.172938439713015</v>
+        <v>48.069185492425042</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>6</v>
@@ -11704,7 +11704,7 @@
       </c>
       <c r="H60" s="38">
         <f t="shared" si="4"/>
-        <v>5.483506009747229</v>
+        <v>14.510601460775927</v>
       </c>
       <c r="I60" s="38">
         <f t="shared" si="7"/>
@@ -11712,11 +11712,11 @@
       </c>
       <c r="J60" s="38">
         <f t="shared" si="5"/>
-        <v>7.8347224615492452</v>
+        <v>15.676307911887713</v>
       </c>
       <c r="K60" s="38">
         <f t="shared" si="3"/>
-        <v>0.69989792703683285</v>
+        <v>0.925638966926147</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -11734,7 +11734,7 @@
       </c>
       <c r="E61" s="34">
         <f t="shared" si="2"/>
-        <v>38.839901343824032</v>
+        <v>47.440561202121479</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>6</v>
@@ -11745,7 +11745,7 @@
       </c>
       <c r="H61" s="38">
         <f t="shared" si="4"/>
-        <v>4.7523718751142656</v>
+        <v>13.474129927863361</v>
       </c>
       <c r="I61" s="38">
         <f t="shared" si="7"/>
@@ -11753,11 +11753,11 @@
       </c>
       <c r="J61" s="38">
         <f t="shared" si="5"/>
-        <v>7.4834261333426859</v>
+        <v>14.928000203895737</v>
       </c>
       <c r="K61" s="38">
         <f t="shared" si="3"/>
-        <v>0.63505295441347309</v>
+        <v>0.90260783385754773</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
       </c>
       <c r="E62" s="34">
         <f t="shared" si="2"/>
-        <v>43.65718069709132</v>
+        <v>48.391034243608232</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>6</v>
@@ -11786,7 +11786,7 @@
       </c>
       <c r="H62" s="38">
         <f t="shared" si="4"/>
-        <v>5.0253889584323579</v>
+        <v>12.997406361587403</v>
       </c>
       <c r="I62" s="38">
         <f t="shared" si="7"/>
@@ -11794,11 +11794,11 @@
       </c>
       <c r="J62" s="38">
         <f t="shared" si="5"/>
-        <v>6.4856359822303284</v>
+        <v>13.861714475046041</v>
       </c>
       <c r="K62" s="38">
         <f t="shared" si="3"/>
-        <v>0.77484906217388261</v>
+        <v>0.93764782018742554</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -11816,7 +11816,7 @@
       </c>
       <c r="E63" s="34">
         <f t="shared" si="2"/>
-        <v>52.166301107745269</v>
+        <v>50.286085122221721</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>6</v>
@@ -11827,7 +11827,7 @@
       </c>
       <c r="H63" s="38">
         <f t="shared" si="4"/>
-        <v>6.1300037639747034</v>
+        <v>13.01973447861687</v>
       </c>
       <c r="I63" s="38">
         <f t="shared" si="7"/>
@@ -11835,11 +11835,11 @@
       </c>
       <c r="J63" s="38">
         <f t="shared" si="5"/>
-        <v>5.6208845179329519</v>
+        <v>12.871592012542752</v>
       </c>
       <c r="K63" s="38">
         <f t="shared" si="3"/>
-        <v>1.0905763575852607</v>
+        <v>1.01150925743527</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -11857,7 +11857,7 @@
       </c>
       <c r="E64" s="34">
         <f t="shared" si="2"/>
-        <v>53.386847845253548</v>
+        <v>50.579740100087569</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>6</v>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="H64" s="38">
         <f t="shared" si="4"/>
-        <v>5.5793365954447429</v>
+        <v>12.232610587287095</v>
       </c>
       <c r="I64" s="38">
         <f t="shared" si="7"/>
@@ -11876,11 +11876,11 @@
       </c>
       <c r="J64" s="38">
         <f t="shared" si="5"/>
-        <v>4.871433248875225</v>
+        <v>11.952192583075414</v>
       </c>
       <c r="K64" s="38">
         <f t="shared" si="3"/>
-        <v>1.145317262990921</v>
+        <v>1.0234616370396139</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="E65" s="34">
         <f t="shared" si="2"/>
-        <v>53.448523579566491</v>
+        <v>50.593882962707148</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>6</v>
@@ -11909,7 +11909,7 @@
       </c>
       <c r="H65" s="38">
         <f t="shared" si="4"/>
-        <v>4.8474250493854631</v>
+        <v>11.365281259623741</v>
       </c>
       <c r="I65" s="38">
         <f t="shared" si="7"/>
@@ -11917,11 +11917,11 @@
       </c>
       <c r="J65" s="38">
         <f t="shared" si="5"/>
-        <v>4.2219088156918616</v>
+        <v>11.098464541427171</v>
       </c>
       <c r="K65" s="38">
         <f t="shared" si="3"/>
-        <v>1.1481595792331425</v>
+        <v>1.0240408677435175</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -11939,7 +11939,7 @@
       </c>
       <c r="E66" s="34">
         <f t="shared" si="2"/>
-        <v>63.647948471932835</v>
+        <v>53.24216578576322</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>6</v>
@@ -11950,7 +11950,7 @@
       </c>
       <c r="H66" s="38">
         <f t="shared" si="4"/>
-        <v>6.4064350428007302</v>
+        <v>11.734904026793471</v>
       </c>
       <c r="I66" s="38">
         <f t="shared" si="7"/>
@@ -11958,11 +11958,11 @@
       </c>
       <c r="J66" s="38">
         <f t="shared" si="5"/>
-        <v>3.6589876402662802</v>
+        <v>10.305717074182374</v>
       </c>
       <c r="K66" s="38">
         <f t="shared" si="3"/>
-        <v>1.7508763823904325</v>
+        <v>1.1386790402185076</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -11980,7 +11980,7 @@
       </c>
       <c r="E67" s="34">
         <f t="shared" si="2"/>
-        <v>69.392775333332693</v>
+        <v>55.163754435840907</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>6</v>
@@ -11991,7 +11991,7 @@
       </c>
       <c r="H67" s="38">
         <f t="shared" si="4"/>
-        <v>7.1895770370939625</v>
+        <v>11.773839453451078</v>
       </c>
       <c r="I67" s="38">
         <f t="shared" ref="I67:I98" si="9">IF(C66&gt;C67,C66-C67,0)</f>
@@ -11999,11 +11999,11 @@
       </c>
       <c r="J67" s="38">
         <f t="shared" si="5"/>
-        <v>3.1711226215641095</v>
+        <v>9.5695944260264891</v>
       </c>
       <c r="K67" s="38">
         <f t="shared" ref="K67:K111" si="10">H67/J67</f>
-        <v>2.2672024689943431</v>
+        <v>1.2303383956826519</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -12021,7 +12021,7 @@
       </c>
       <c r="E68" s="34">
         <f t="shared" si="2"/>
-        <v>71.563184608167234</v>
+        <v>55.979233975902638</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>6</v>
@@ -12032,7 +12032,7 @@
       </c>
       <c r="H68" s="38">
         <f t="shared" si="4"/>
-        <v>6.9163000988147809</v>
+        <v>11.299993778204581</v>
       </c>
       <c r="I68" s="38">
         <f t="shared" si="9"/>
@@ -12040,11 +12040,11 @@
       </c>
       <c r="J68" s="38">
         <f t="shared" si="5"/>
-        <v>2.7483062720222282</v>
+        <v>8.8860519670245974</v>
       </c>
       <c r="K68" s="38">
         <f t="shared" si="10"/>
-        <v>2.5165681748147035</v>
+        <v>1.271655153507758</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -12062,7 +12062,7 @@
       </c>
       <c r="E69" s="34">
         <f t="shared" si="2"/>
-        <v>65.600451010230984</v>
+        <v>54.787114103815249</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>6</v>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="H69" s="38">
         <f t="shared" si="4"/>
-        <v>5.9941267523061432</v>
+        <v>10.492851365475682</v>
       </c>
       <c r="I69" s="38">
         <f t="shared" si="9"/>
@@ -12081,11 +12081,11 @@
       </c>
       <c r="J69" s="38">
         <f t="shared" si="5"/>
-        <v>3.1431987690859362</v>
+        <v>8.6591911122371279</v>
       </c>
       <c r="K69" s="38">
         <f t="shared" si="10"/>
-        <v>1.9070148573675079</v>
+        <v>1.2117588386110607</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -12103,7 +12103,7 @@
       </c>
       <c r="E70" s="34">
         <f t="shared" si="2"/>
-        <v>68.058229459379092</v>
+        <v>55.602044879818095</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>6</v>
@@ -12114,7 +12114,7 @@
       </c>
       <c r="H70" s="38">
         <f t="shared" si="4"/>
-        <v>5.8042431853319822</v>
+        <v>10.069790553655986</v>
       </c>
       <c r="I70" s="38">
         <f t="shared" si="9"/>
@@ -12122,11 +12122,11 @@
       </c>
       <c r="J70" s="38">
         <f t="shared" si="5"/>
-        <v>2.7241055998744783</v>
+        <v>8.0406774613630478</v>
       </c>
       <c r="K70" s="38">
         <f t="shared" si="10"/>
-        <v>2.1306968370093404</v>
+        <v>1.2523559864256717</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -12144,7 +12144,7 @@
       </c>
       <c r="E71" s="34">
         <f t="shared" si="2"/>
-        <v>72.777483416154524</v>
+        <v>57.343204507429149</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>6</v>
@@ -12155,7 +12155,7 @@
       </c>
       <c r="H71" s="38">
         <f t="shared" si="4"/>
-        <v>6.3116774272877052</v>
+        <v>10.036948371251981</v>
       </c>
       <c r="I71" s="38">
         <f t="shared" si="9"/>
@@ -12163,11 +12163,11 @@
       </c>
       <c r="J71" s="38">
         <f t="shared" si="5"/>
-        <v>2.3608915198912146</v>
+        <v>7.4663433569799738</v>
       </c>
       <c r="K71" s="38">
         <f t="shared" si="10"/>
-        <v>2.6734296659164309</v>
+        <v>1.3442923652672436</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -12185,7 +12185,7 @@
       </c>
       <c r="E72" s="34">
         <f t="shared" si="2"/>
-        <v>75.84545144464478</v>
+        <v>58.644521174846872</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>6</v>
@@ -12196,7 +12196,7 @@
       </c>
       <c r="H72" s="38">
         <f t="shared" si="4"/>
-        <v>6.424787103649356</v>
+        <v>9.8314520590197017</v>
       </c>
       <c r="I72" s="38">
         <f t="shared" si="9"/>
@@ -12204,11 +12204,11 @@
       </c>
       <c r="J72" s="38">
         <f t="shared" si="5"/>
-        <v>2.0461059839057194</v>
+        <v>6.9330331171956905</v>
       </c>
       <c r="K72" s="38">
         <f t="shared" si="10"/>
-        <v>3.1400069958181587</v>
+        <v>1.4180592956689033</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -12226,7 +12226,7 @@
       </c>
       <c r="E73" s="34">
         <f t="shared" si="2"/>
-        <v>82.459050806351925</v>
+        <v>62.241277893210373</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>6</v>
@@ -12237,7 +12237,7 @@
       </c>
       <c r="H73" s="38">
         <f t="shared" si="4"/>
-        <v>8.3361488231627732</v>
+        <v>10.61206262623258</v>
       </c>
       <c r="I73" s="38">
         <f t="shared" si="9"/>
@@ -12245,11 +12245,11 @@
       </c>
       <c r="J73" s="38">
         <f t="shared" si="5"/>
-        <v>1.7732918527182902</v>
+        <v>6.4378164659674271</v>
       </c>
       <c r="K73" s="38">
         <f t="shared" si="10"/>
-        <v>4.7009457638821486</v>
+        <v>1.6483947130726224</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -12267,7 +12267,7 @@
       </c>
       <c r="E74" s="34">
         <f t="shared" si="2"/>
-        <v>78.652771400017727</v>
+        <v>61.360929863887428</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>6</v>
@@ -12278,7 +12278,7 @@
       </c>
       <c r="H74" s="38">
         <f t="shared" si="4"/>
-        <v>7.2246623134077366</v>
+        <v>9.8540581529302536</v>
       </c>
       <c r="I74" s="38">
         <f t="shared" si="9"/>
@@ -12286,11 +12286,11 @@
       </c>
       <c r="J74" s="38">
         <f t="shared" si="5"/>
-        <v>1.9608529390225269</v>
+        <v>6.2051152898269013</v>
       </c>
       <c r="K74" s="38">
         <f t="shared" si="10"/>
-        <v>3.6844488281763681</v>
+        <v>1.5880539994294198</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -12308,7 +12308,7 @@
       </c>
       <c r="E75" s="34">
         <f t="shared" si="2"/>
-        <v>65.099815967359021</v>
+        <v>57.912833444891852</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>6</v>
@@ -12319,7 +12319,7 @@
       </c>
       <c r="H75" s="38">
         <f t="shared" si="4"/>
-        <v>6.2613740049533719</v>
+        <v>9.1501968562923786</v>
       </c>
       <c r="I75" s="38">
         <f t="shared" si="9"/>
@@ -12327,11 +12327,11 @@
       </c>
       <c r="J75" s="38">
         <f t="shared" si="5"/>
-        <v>3.3567392138195018</v>
+        <v>6.6497499119821111</v>
       </c>
       <c r="K75" s="38">
         <f t="shared" si="10"/>
-        <v>1.8653144036854743</v>
+        <v>1.3760212004070618</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -12349,7 +12349,7 @@
       </c>
       <c r="E76" s="34">
         <f t="shared" si="2"/>
-        <v>57.657226854755351</v>
+        <v>55.723494985390673</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>6</v>
@@ -12360,7 +12360,7 @@
       </c>
       <c r="H76" s="38">
         <f t="shared" si="4"/>
-        <v>5.4265241376262559</v>
+        <v>8.4966113665572092</v>
       </c>
       <c r="I76" s="38">
         <f t="shared" si="9"/>
@@ -12368,11 +12368,11 @@
       </c>
       <c r="J76" s="38">
         <f t="shared" si="5"/>
-        <v>3.985173985310257</v>
+        <v>6.7511963468405431</v>
       </c>
       <c r="K76" s="38">
         <f t="shared" si="10"/>
-        <v>1.3616780992822288</v>
+        <v>1.2585341812097486</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -12390,7 +12390,7 @@
       </c>
       <c r="E77" s="34">
         <f t="shared" si="2"/>
-        <v>53.772160755510612</v>
+        <v>54.508058623627754</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>6</v>
@@ -12401,7 +12401,7 @@
       </c>
       <c r="H77" s="38">
         <f t="shared" si="4"/>
-        <v>4.702987585942755</v>
+        <v>7.8897105546602662</v>
       </c>
       <c r="I77" s="38">
         <f t="shared" si="9"/>
@@ -12409,11 +12409,11 @@
       </c>
       <c r="J77" s="38">
         <f t="shared" si="5"/>
-        <v>4.0431507872688686</v>
+        <v>6.5846823220662074</v>
       </c>
       <c r="K77" s="38">
         <f t="shared" si="10"/>
-        <v>1.163198661982034</v>
+        <v>1.1981915252343645</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="E78" s="34">
         <f t="shared" si="2"/>
-        <v>49.706454147087669</v>
+        <v>53.193535882253848</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>6</v>
@@ -12442,7 +12442,7 @@
       </c>
       <c r="H78" s="38">
         <f t="shared" si="4"/>
-        <v>4.0759225744837213</v>
+        <v>7.3261598007559616</v>
       </c>
       <c r="I78" s="38">
         <f t="shared" si="9"/>
@@ -12450,11 +12450,11 @@
       </c>
       <c r="J78" s="38">
         <f t="shared" si="5"/>
-        <v>4.1240640156330315</v>
+        <v>6.4464907276329138</v>
       </c>
       <c r="K78" s="38">
         <f t="shared" si="10"/>
-        <v>0.98832669886625879</v>
+        <v>1.1364570446603361</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -12472,7 +12472,7 @@
       </c>
       <c r="E79" s="34">
         <f t="shared" si="2"/>
-        <v>54.718825049650043</v>
+        <v>54.686730882362639</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>6</v>
@@ -12483,7 +12483,7 @@
       </c>
       <c r="H79" s="38">
         <f t="shared" si="4"/>
-        <v>4.319132897885904</v>
+        <v>7.2242912435591142</v>
       </c>
       <c r="I79" s="38">
         <f t="shared" si="9"/>
@@ -12491,11 +12491,11 @@
       </c>
       <c r="J79" s="38">
         <f t="shared" si="5"/>
-        <v>3.5741888135486275</v>
+        <v>5.9860271042305628</v>
       </c>
       <c r="K79" s="38">
         <f t="shared" si="10"/>
-        <v>1.2084232599893512</v>
+        <v>1.2068590933130625</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -12513,7 +12513,7 @@
       </c>
       <c r="E80" s="34">
         <f t="shared" ref="E80:E111" si="11">100-(100 / (1 + K80))</f>
-        <v>48.215709170255948</v>
+        <v>52.568491804117556</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>6</v>
@@ -12524,7 +12524,7 @@
       </c>
       <c r="H80" s="38">
         <f t="shared" si="4"/>
-        <v>3.7432485115011169</v>
+        <v>6.7082704404477491</v>
       </c>
       <c r="I80" s="38">
         <f t="shared" si="9"/>
@@ -12532,11 +12532,11 @@
       </c>
       <c r="J80" s="38">
         <f t="shared" si="5"/>
-        <v>4.0202969717421535</v>
+        <v>6.0527394539283845</v>
       </c>
       <c r="K80" s="38">
         <f t="shared" si="10"/>
-        <v>0.93108756338440823</v>
+        <v>1.1083031892433282</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -12554,7 +12554,7 @@
       </c>
       <c r="E81" s="34">
         <f t="shared" si="11"/>
-        <v>40.108628024901066</v>
+        <v>49.523519972547057</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>6</v>
@@ -12564,20 +12564,20 @@
         <v>0</v>
       </c>
       <c r="H81" s="38">
-        <f t="shared" ref="H81:H111" si="12">G81*2/(14+1)+H80*(1-2/(14+1))</f>
-        <v>3.2441487099676349</v>
+        <f t="shared" si="4"/>
+        <v>6.2291082661300532</v>
       </c>
       <c r="I81" s="38">
         <f t="shared" si="9"/>
         <v>10.200000000000045</v>
       </c>
       <c r="J81" s="38">
-        <f t="shared" ref="J81:J111" si="13">I81*2/(14+1)+J80*(1-2/(14+1))</f>
-        <v>4.8442573755098728</v>
+        <f t="shared" si="5"/>
+        <v>6.3489723500763597</v>
       </c>
       <c r="K81" s="38">
         <f t="shared" si="10"/>
-        <v>0.66968958469639084</v>
+        <v>0.98112071098484699</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -12595,7 +12595,7 @@
       </c>
       <c r="E82" s="34">
         <f t="shared" si="11"/>
-        <v>52.30920887603444</v>
+        <v>53.359919668425192</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>6</v>
@@ -12605,20 +12605,20 @@
         <v>13.450000000000045</v>
       </c>
       <c r="H82" s="38">
-        <f t="shared" si="12"/>
-        <v>4.604928881971956</v>
+        <f t="shared" ref="H82:H111" si="12">((H81*13)+G82)/14</f>
+        <v>6.7448862471207667</v>
       </c>
       <c r="I82" s="38">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J82" s="38">
-        <f t="shared" si="13"/>
-        <v>4.1983563921085567</v>
+        <f t="shared" ref="J82:J111" si="13">((J81*13)+I82)/14</f>
+        <v>5.8954743250709054</v>
       </c>
       <c r="K82" s="38">
         <f t="shared" si="10"/>
-        <v>1.0968408710198148</v>
+        <v>1.1440786398539096</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="E83" s="34">
         <f t="shared" si="11"/>
-        <v>51.296217716570617</v>
+        <v>52.995489321006112</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>6</v>
@@ -12647,7 +12647,7 @@
       </c>
       <c r="H83" s="38">
         <f t="shared" si="12"/>
-        <v>3.9909383643756953</v>
+        <v>6.2631086580407125</v>
       </c>
       <c r="I83" s="38">
         <f t="shared" si="9"/>
@@ -12655,11 +12655,11 @@
       </c>
       <c r="J83" s="38">
         <f t="shared" si="13"/>
-        <v>3.7892422064940972</v>
+        <v>5.5550833018515622</v>
       </c>
       <c r="K83" s="38">
         <f t="shared" si="10"/>
-        <v>1.0532286264351025</v>
+        <v>1.1274553985451774</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -12677,7 +12677,7 @@
       </c>
       <c r="E84" s="34">
         <f t="shared" si="11"/>
-        <v>39.435446200074075</v>
+        <v>48.221559069817339</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>6</v>
@@ -12688,7 +12688,7 @@
       </c>
       <c r="H84" s="38">
         <f t="shared" si="12"/>
-        <v>3.4588132491256025</v>
+        <v>5.8157437538949477</v>
       </c>
       <c r="I84" s="38">
         <f t="shared" si="9"/>
@@ -12696,11 +12696,11 @@
       </c>
       <c r="J84" s="38">
         <f t="shared" si="13"/>
-        <v>5.312009912294859</v>
+        <v>6.2447202088621507</v>
       </c>
       <c r="K84" s="38">
         <f t="shared" si="10"/>
-        <v>0.65113079723741496</v>
+        <v>0.93130573658713733</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -12718,7 +12718,7 @@
       </c>
       <c r="E85" s="34">
         <f t="shared" si="11"/>
-        <v>49.85056117437405</v>
+        <v>51.857158716576279</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>6</v>
@@ -12729,7 +12729,7 @@
       </c>
       <c r="H85" s="38">
         <f t="shared" si="12"/>
-        <v>4.5763048159088449</v>
+        <v>6.246047771473874</v>
       </c>
       <c r="I85" s="38">
         <f t="shared" si="9"/>
@@ -12737,11 +12737,11 @@
       </c>
       <c r="J85" s="38">
         <f t="shared" si="13"/>
-        <v>4.6037419239888777</v>
+        <v>5.798668765371997</v>
       </c>
       <c r="K85" s="38">
         <f t="shared" si="10"/>
-        <v>0.99404025930796303</v>
+        <v>1.0771520195761994</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -12759,7 +12759,7 @@
       </c>
       <c r="E86" s="34">
         <f t="shared" si="11"/>
-        <v>40.169965244163528</v>
+        <v>47.495318481339517</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>6</v>
@@ -12770,7 +12770,7 @@
       </c>
       <c r="H86" s="38">
         <f t="shared" si="12"/>
-        <v>3.9661308404543325</v>
+        <v>5.799901502082883</v>
       </c>
       <c r="I86" s="38">
         <f t="shared" si="9"/>
@@ -12778,11 +12778,11 @@
       </c>
       <c r="J86" s="38">
         <f t="shared" si="13"/>
-        <v>5.9072430007903751</v>
+        <v>6.4116209964168629</v>
       </c>
       <c r="K86" s="38">
         <f t="shared" si="10"/>
-        <v>0.67140133560167981</v>
+        <v>0.9045920688893121</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -12800,7 +12800,7 @@
       </c>
       <c r="E87" s="34">
         <f t="shared" si="11"/>
-        <v>30.383951985827352</v>
+        <v>42.023635455532883</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>6</v>
@@ -12811,7 +12811,7 @@
       </c>
       <c r="H87" s="38">
         <f t="shared" si="12"/>
-        <v>3.4373133950604218</v>
+        <v>5.3856228233626764</v>
       </c>
       <c r="I87" s="38">
         <f t="shared" si="9"/>
@@ -12819,11 +12819,11 @@
       </c>
       <c r="J87" s="38">
         <f t="shared" si="13"/>
-        <v>7.875610600684972</v>
+        <v>7.4300766395299336</v>
       </c>
       <c r="K87" s="38">
         <f t="shared" si="10"/>
-        <v>0.43645039976474531</v>
+        <v>0.72484081721442373</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -12841,7 +12841,7 @@
       </c>
       <c r="E88" s="34">
         <f t="shared" si="11"/>
-        <v>31.271864024796116</v>
+        <v>42.352350471235063</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>6</v>
@@ -12852,7 +12852,7 @@
       </c>
       <c r="H88" s="38">
         <f t="shared" si="12"/>
-        <v>3.1056716090523717</v>
+        <v>5.068792621693917</v>
       </c>
       <c r="I88" s="38">
         <f t="shared" si="9"/>
@@ -12860,11 +12860,11 @@
       </c>
       <c r="J88" s="38">
         <f t="shared" si="13"/>
-        <v>6.825529187260309</v>
+        <v>6.8993568795635101</v>
       </c>
       <c r="K88" s="38">
         <f t="shared" si="10"/>
-        <v>0.45500817941692129</v>
+        <v>0.73467610245066717</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -12882,7 +12882,7 @@
       </c>
       <c r="E89" s="34">
         <f t="shared" si="11"/>
-        <v>55.948064757359916</v>
+        <v>53.22370956615341</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>6</v>
@@ -12893,7 +12893,7 @@
       </c>
       <c r="H89" s="38">
         <f t="shared" si="12"/>
-        <v>7.5129153945120368</v>
+        <v>7.2895931487157695</v>
       </c>
       <c r="I89" s="38">
         <f t="shared" si="9"/>
@@ -12901,11 +12901,11 @@
       </c>
       <c r="J89" s="38">
         <f t="shared" si="13"/>
-        <v>5.9154586289589348</v>
+        <v>6.4065456738804025</v>
       </c>
       <c r="K89" s="38">
         <f t="shared" si="10"/>
-        <v>1.2700478298897746</v>
+        <v>1.137835195405781</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -12923,7 +12923,7 @@
       </c>
       <c r="E90" s="34">
         <f t="shared" si="11"/>
-        <v>60.734537198047001</v>
+        <v>55.861370519928386</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>6</v>
@@ -12934,7 +12934,7 @@
       </c>
       <c r="H90" s="38">
         <f t="shared" si="12"/>
-        <v>7.929860008577112</v>
+        <v>7.5289079238075072</v>
       </c>
       <c r="I90" s="38">
         <f t="shared" si="9"/>
@@ -12942,11 +12942,11 @@
       </c>
       <c r="J90" s="38">
         <f t="shared" si="13"/>
-        <v>5.1267308117644106</v>
+        <v>5.9489352686032309</v>
       </c>
       <c r="K90" s="38">
         <f t="shared" si="10"/>
-        <v>1.5467673844665895</v>
+        <v>1.2655891489596327</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -12964,7 +12964,7 @@
       </c>
       <c r="E91" s="34">
         <f t="shared" si="11"/>
-        <v>63.702718465131234</v>
+        <v>57.543054790945398</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>6</v>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="H91" s="38">
         <f t="shared" si="12"/>
-        <v>7.7978786741001711</v>
+        <v>7.4868430721069741</v>
       </c>
       <c r="I91" s="38">
         <f t="shared" si="9"/>
@@ -12983,11 +12983,11 @@
       </c>
       <c r="J91" s="38">
         <f t="shared" si="13"/>
-        <v>4.4431667035291564</v>
+        <v>5.5240113208458572</v>
       </c>
       <c r="K91" s="38">
         <f t="shared" si="10"/>
-        <v>1.7550272574527543</v>
+        <v>1.3553272499377429</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -13005,7 +13005,7 @@
       </c>
       <c r="E92" s="34">
         <f t="shared" si="11"/>
-        <v>55.306038150886948</v>
+        <v>53.707297946910209</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>6</v>
@@ -13016,7 +13016,7 @@
       </c>
       <c r="H92" s="38">
         <f t="shared" si="12"/>
-        <v>6.7581615175534822</v>
+        <v>6.9520685669564761</v>
       </c>
       <c r="I92" s="38">
         <f t="shared" si="9"/>
@@ -13024,11 +13024,11 @@
       </c>
       <c r="J92" s="38">
         <f t="shared" si="13"/>
-        <v>5.4614111430586227</v>
+        <v>5.992296226499735</v>
       </c>
       <c r="K92" s="38">
         <f t="shared" si="10"/>
-        <v>1.2374387022927236</v>
+        <v>1.1601677060310103</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -13046,7 +13046,7 @@
       </c>
       <c r="E93" s="34">
         <f t="shared" si="11"/>
-        <v>65.503711363941676</v>
+        <v>59.375691303433747</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>6</v>
@@ -13057,7 +13057,7 @@
       </c>
       <c r="H93" s="38">
         <f t="shared" si="12"/>
-        <v>8.9877399818796881</v>
+        <v>8.1326350978881585</v>
       </c>
       <c r="I93" s="38">
         <f t="shared" si="9"/>
@@ -13065,11 +13065,11 @@
       </c>
       <c r="J93" s="38">
         <f t="shared" si="13"/>
-        <v>4.7332229906508063</v>
+        <v>5.5642750674640391</v>
       </c>
       <c r="K93" s="38">
         <f t="shared" si="10"/>
-        <v>1.8988625720006267</v>
+        <v>1.4615803495125681</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
       </c>
       <c r="E94" s="34">
         <f t="shared" si="11"/>
-        <v>69.477092060415785</v>
+        <v>61.86237154468153</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>6</v>
@@ -13098,7 +13098,7 @@
       </c>
       <c r="H94" s="38">
         <f t="shared" si="12"/>
-        <v>9.3373746509624134</v>
+        <v>8.3810183051818701</v>
       </c>
       <c r="I94" s="38">
         <f t="shared" si="9"/>
@@ -13106,11 +13106,11 @@
       </c>
       <c r="J94" s="38">
         <f t="shared" si="13"/>
-        <v>4.1021265918973659</v>
+        <v>5.1668268483594648</v>
       </c>
       <c r="K94" s="38">
         <f t="shared" si="10"/>
-        <v>2.2762278154472009</v>
+        <v>1.6220822859281521</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -13128,7 +13128,7 @@
       </c>
       <c r="E95" s="34">
         <f t="shared" si="11"/>
-        <v>72.986831533760181</v>
+        <v>64.171314282761173</v>
       </c>
       <c r="F95" s="5" t="s">
         <v>6</v>
@@ -13139,7 +13139,7 @@
       </c>
       <c r="H95" s="38">
         <f t="shared" si="12"/>
-        <v>9.6057246975007455</v>
+        <v>8.5930884262403016</v>
       </c>
       <c r="I95" s="38">
         <f t="shared" si="9"/>
@@ -13147,11 +13147,11 @@
       </c>
       <c r="J95" s="38">
         <f t="shared" si="13"/>
-        <v>3.5551763796443838</v>
+        <v>4.7977677877623606</v>
       </c>
       <c r="K95" s="38">
         <f t="shared" si="10"/>
-        <v>2.7018982103109002</v>
+        <v>1.7910596774105334</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -13169,7 +13169,7 @@
       </c>
       <c r="E96" s="34">
         <f t="shared" si="11"/>
-        <v>73.037261073885162</v>
+        <v>64.204214607093505</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>6</v>
@@ -13180,7 +13180,7 @@
       </c>
       <c r="H96" s="38">
         <f t="shared" si="12"/>
-        <v>8.3462947378339898</v>
+        <v>7.9907249672231435</v>
       </c>
       <c r="I96" s="38">
         <f t="shared" si="9"/>
@@ -13188,11 +13188,11 @@
       </c>
       <c r="J96" s="38">
         <f t="shared" si="13"/>
-        <v>3.0811528623584663</v>
+        <v>4.4550700886364778</v>
       </c>
       <c r="K96" s="38">
         <f t="shared" si="10"/>
-        <v>2.7088220256119731</v>
+        <v>1.7936249729504909</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
       </c>
       <c r="E97" s="34">
         <f t="shared" si="11"/>
-        <v>76.239326678962357</v>
+        <v>66.289806479246295</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>6</v>
@@ -13221,7 +13221,7 @@
       </c>
       <c r="H97" s="38">
         <f t="shared" si="12"/>
-        <v>8.5681221061227912</v>
+        <v>8.1349588981357748</v>
       </c>
       <c r="I97" s="38">
         <f t="shared" si="9"/>
@@ -13229,11 +13229,11 @@
       </c>
       <c r="J97" s="38">
         <f t="shared" si="13"/>
-        <v>2.670332480710671</v>
+        <v>4.1368507965910153</v>
       </c>
       <c r="K97" s="38">
         <f t="shared" si="10"/>
-        <v>3.2086349426579672</v>
+        <v>1.9664617599550394</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -13251,7 +13251,7 @@
       </c>
       <c r="E98" s="34">
         <f t="shared" si="11"/>
-        <v>68.469172151453691</v>
+        <v>63.015280501225966</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>6</v>
@@ -13262,7 +13262,7 @@
       </c>
       <c r="H98" s="38">
         <f t="shared" si="12"/>
-        <v>7.4257058253064194</v>
+        <v>7.5538904054117912</v>
       </c>
       <c r="I98" s="38">
         <f t="shared" si="9"/>
@@ -13270,11 +13270,11 @@
       </c>
       <c r="J98" s="38">
         <f t="shared" si="13"/>
-        <v>3.4196214832825769</v>
+        <v>4.4335043111202257</v>
       </c>
       <c r="K98" s="38">
         <f t="shared" si="10"/>
-        <v>2.1714993491555403</v>
+        <v>1.7038193436431166</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -13292,7 +13292,7 @@
       </c>
       <c r="E99" s="34">
         <f t="shared" si="11"/>
-        <v>70.82411456348423</v>
+        <v>64.318122662026127</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>6</v>
@@ -13303,7 +13303,7 @@
       </c>
       <c r="H99" s="38">
         <f t="shared" si="12"/>
-        <v>7.1942783819322074</v>
+        <v>7.4207553764537932</v>
       </c>
       <c r="I99" s="38">
         <f t="shared" ref="I99:I111" si="15">IF(C98&gt;C99,C98-C99,0)</f>
@@ -13311,11 +13311,11 @@
       </c>
       <c r="J99" s="38">
         <f t="shared" si="13"/>
-        <v>2.9636719521782333</v>
+        <v>4.1168254317544948</v>
       </c>
       <c r="K99" s="38">
         <f t="shared" si="10"/>
-        <v>2.427488095180228</v>
+        <v>1.8025431244217807</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -13333,7 +13333,7 @@
       </c>
       <c r="E100" s="34">
         <f t="shared" si="11"/>
-        <v>73.871238433422477</v>
+        <v>66.06048413734905</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>6</v>
@@ -13344,7 +13344,7 @@
       </c>
       <c r="H100" s="38">
         <f t="shared" si="12"/>
-        <v>7.2617079310079191</v>
+        <v>7.4407014209928111</v>
       </c>
       <c r="I100" s="38">
         <f t="shared" si="15"/>
@@ -13352,11 +13352,11 @@
       </c>
       <c r="J100" s="38">
         <f t="shared" si="13"/>
-        <v>2.5685156918878023</v>
+        <v>3.8227664723434596</v>
       </c>
       <c r="K100" s="38">
         <f t="shared" si="10"/>
-        <v>2.8272001428462072</v>
+        <v>1.9464179867705753</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -13374,7 +13374,7 @@
       </c>
       <c r="E101" s="34">
         <f t="shared" si="11"/>
-        <v>74.794314757560556</v>
+        <v>66.59433566839013</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>6</v>
@@ -13385,7 +13385,7 @@
       </c>
       <c r="H101" s="38">
         <f t="shared" si="12"/>
-        <v>6.6054802068735192</v>
+        <v>7.0763656052076049</v>
       </c>
       <c r="I101" s="38">
         <f t="shared" si="15"/>
@@ -13393,11 +13393,11 @@
       </c>
       <c r="J101" s="38">
         <f t="shared" si="13"/>
-        <v>2.2260469329694286</v>
+        <v>3.5497117243189265</v>
       </c>
       <c r="K101" s="38">
         <f t="shared" si="10"/>
-        <v>2.9673589128069997</v>
+        <v>1.9935043053574522</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -13415,7 +13415,7 @@
       </c>
       <c r="E102" s="34">
         <f t="shared" si="11"/>
-        <v>78.482681390265924</v>
+        <v>68.815676029426697</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>6</v>
@@ -13426,7 +13426,7 @@
       </c>
       <c r="H102" s="38">
         <f t="shared" si="12"/>
-        <v>7.0367495126237358</v>
+        <v>7.273768061978501</v>
       </c>
       <c r="I102" s="38">
         <f t="shared" si="15"/>
@@ -13434,11 +13434,11 @@
       </c>
       <c r="J102" s="38">
         <f t="shared" si="13"/>
-        <v>1.9292406752401714</v>
+        <v>3.2961608868675745</v>
       </c>
       <c r="K102" s="38">
         <f t="shared" si="10"/>
-        <v>3.6474192167588058</v>
+        <v>2.2067393891355067</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -13456,7 +13456,7 @@
       </c>
       <c r="E103" s="34">
         <f t="shared" si="11"/>
-        <v>68.349669637488802</v>
+        <v>64.744664724086633</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>6</v>
@@ -13467,7 +13467,7 @@
       </c>
       <c r="H103" s="38">
         <f t="shared" si="12"/>
-        <v>6.0985162442739043</v>
+        <v>6.754213200408608</v>
       </c>
       <c r="I103" s="38">
         <f t="shared" si="15"/>
@@ -13475,11 +13475,11 @@
       </c>
       <c r="J103" s="38">
         <f t="shared" si="13"/>
-        <v>2.824008585208162</v>
+        <v>3.6778636806627545</v>
       </c>
       <c r="K103" s="38">
         <f t="shared" si="10"/>
-        <v>2.1595246828275392</v>
+        <v>1.836450120737344</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -13497,7 +13497,7 @@
       </c>
       <c r="E104" s="34">
         <f t="shared" si="11"/>
-        <v>61.205113477849963</v>
+        <v>61.66628410041254</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>6</v>
@@ -13508,7 +13508,7 @@
       </c>
       <c r="H104" s="38">
         <f t="shared" si="12"/>
-        <v>5.2853807450373838</v>
+        <v>6.2717694003794211</v>
       </c>
       <c r="I104" s="38">
         <f t="shared" si="15"/>
@@ -13516,11 +13516,11 @@
       </c>
       <c r="J104" s="38">
         <f t="shared" si="13"/>
-        <v>3.3501407738470714</v>
+        <v>3.8987305606154132</v>
       </c>
       <c r="K104" s="38">
         <f t="shared" si="10"/>
-        <v>1.5776592990652198</v>
+        <v>1.6086696176792028</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -13538,7 +13538,7 @@
       </c>
       <c r="E105" s="34">
         <f t="shared" si="11"/>
-        <v>64.436389745011084</v>
+        <v>63.090016512830772</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>6</v>
@@ -13549,7 +13549,7 @@
       </c>
       <c r="H105" s="38">
         <f t="shared" si="12"/>
-        <v>5.2606633123657511</v>
+        <v>6.1880715860666147</v>
       </c>
       <c r="I105" s="38">
         <f t="shared" si="15"/>
@@ -13557,11 +13557,11 @@
       </c>
       <c r="J105" s="38">
         <f t="shared" si="13"/>
-        <v>2.9034553373341287</v>
+        <v>3.6202498062857411</v>
       </c>
       <c r="K105" s="38">
         <f t="shared" si="10"/>
-        <v>1.811863004993197</v>
+        <v>1.7092940866462956</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -13579,7 +13579,7 @@
       </c>
       <c r="E106" s="34">
         <f t="shared" si="11"/>
-        <v>68.20504332731737</v>
+        <v>64.825195567061002</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>6</v>
@@ -13590,7 +13590,7 @@
       </c>
       <c r="H106" s="38">
         <f t="shared" si="12"/>
-        <v>5.3979082040503137</v>
+        <v>6.1953521870618546</v>
       </c>
       <c r="I106" s="38">
         <f t="shared" si="15"/>
@@ -13598,11 +13598,11 @@
       </c>
       <c r="J106" s="38">
         <f t="shared" si="13"/>
-        <v>2.5163279590229117</v>
+        <v>3.361660534408188</v>
       </c>
       <c r="K106" s="38">
         <f t="shared" si="10"/>
-        <v>2.1451528941983846</v>
+        <v>1.8429440223513023</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -13620,7 +13620,7 @@
       </c>
       <c r="E107" s="34">
         <f t="shared" si="11"/>
-        <v>62.207138897245812</v>
+        <v>62.33657273560928</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>6</v>
@@ -13631,7 +13631,7 @@
       </c>
       <c r="H107" s="38">
         <f t="shared" si="12"/>
-        <v>4.678187110176939</v>
+        <v>5.7528270308431511</v>
       </c>
       <c r="I107" s="38">
         <f t="shared" si="15"/>
@@ -13639,11 +13639,11 @@
       </c>
       <c r="J107" s="38">
         <f t="shared" si="13"/>
-        <v>2.8421508978198617</v>
+        <v>3.4758276390933203</v>
       </c>
       <c r="K107" s="38">
         <f t="shared" si="10"/>
-        <v>1.6460023687572154</v>
+        <v>1.655095599718458</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -13661,7 +13661,7 @@
       </c>
       <c r="E108" s="34">
         <f t="shared" si="11"/>
-        <v>67.245990756700778</v>
+        <v>64.558106937522496</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>6</v>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="H108" s="38">
         <f t="shared" si="12"/>
-        <v>5.0570954954866778</v>
+        <v>5.8790536714972106</v>
       </c>
       <c r="I108" s="38">
         <f t="shared" si="15"/>
@@ -13680,11 +13680,11 @@
       </c>
       <c r="J108" s="38">
         <f t="shared" si="13"/>
-        <v>2.4631974447772138</v>
+        <v>3.2275542363009402</v>
       </c>
       <c r="K108" s="38">
         <f t="shared" si="10"/>
-        <v>2.0530613598229319</v>
+        <v>1.8215197146416109</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -13702,7 +13702,7 @@
       </c>
       <c r="E109" s="34">
         <f t="shared" si="11"/>
-        <v>45.514059930927985</v>
+        <v>53.926414451262737</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>6</v>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="H109" s="38">
         <f t="shared" si="12"/>
-        <v>4.3828160960884546</v>
+        <v>5.4591212663902677</v>
       </c>
       <c r="I109" s="38">
         <f t="shared" si="15"/>
@@ -13721,11 +13721,11 @@
       </c>
       <c r="J109" s="38">
         <f t="shared" si="13"/>
-        <v>5.2467711188069082</v>
+        <v>4.6641575051365818</v>
       </c>
       <c r="K109" s="38">
         <f t="shared" si="10"/>
-        <v>0.83533586597257303</v>
+        <v>1.1704410197078898</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -13743,7 +13743,7 @@
       </c>
       <c r="E110" s="34">
         <f t="shared" si="11"/>
-        <v>60.368281178138361</v>
+        <v>60.897058239447965</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>6</v>
@@ -13754,7 +13754,7 @@
       </c>
       <c r="H110" s="38">
         <f t="shared" si="12"/>
-        <v>6.9264406166099679</v>
+        <v>6.7448983187909493</v>
       </c>
       <c r="I110" s="38">
         <f t="shared" si="15"/>
@@ -13762,11 +13762,11 @@
       </c>
       <c r="J110" s="38">
         <f t="shared" si="13"/>
-        <v>4.5472016362993202</v>
+        <v>4.3310033976268256</v>
       </c>
       <c r="K110" s="38">
         <f t="shared" si="10"/>
-        <v>1.5232314664293092</v>
+        <v>1.5573523499166078</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -13784,7 +13784,7 @@
       </c>
       <c r="E111" s="34">
         <f t="shared" si="11"/>
-        <v>61.037006282157336</v>
+        <v>61.241609039909484</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>6</v>
@@ -13795,7 +13795,7 @@
       </c>
       <c r="H111" s="38">
         <f t="shared" si="12"/>
-        <v>6.1735818677286654</v>
+        <v>6.3545484388773241</v>
       </c>
       <c r="I111" s="38">
         <f t="shared" si="15"/>
@@ -13803,11 +13803,11 @@
       </c>
       <c r="J111" s="38">
         <f t="shared" si="13"/>
-        <v>3.9409080847927442</v>
+        <v>4.0216460120820523</v>
       </c>
       <c r="K111" s="38">
         <f t="shared" si="10"/>
-        <v>1.5665378980929314</v>
+        <v>1.5800864670303245</v>
       </c>
     </row>
     <row r="112" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -13833,11 +13833,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W31" sqref="W31"/>
+      <selection pane="bottomRight" activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -52495,7 +52495,7 @@
         <v>46.090461148121541</v>
       </c>
       <c r="V465" s="51">
-        <f t="shared" ref="V465:V528" si="94">(100*(T465/U465))</f>
+        <f t="shared" ref="V465:V506" si="94">(100*(T465/U465))</f>
         <v>27.380240951667229</v>
       </c>
       <c r="W465" s="51">
@@ -53744,7 +53744,7 @@
         <v>16.056204692224895</v>
       </c>
       <c r="W480" s="51">
-        <f t="shared" ref="W480:W543" si="100">((W479*13)+V480)/14</f>
+        <f t="shared" ref="W480:W506" si="100">((W479*13)+V480)/14</f>
         <v>14.880640374767012</v>
       </c>
       <c r="X480" s="43" t="s">

</xml_diff>